<commit_message>
Final commit of day 1
</commit_message>
<xml_diff>
--- a/Ege Zeitplan.xlsx
+++ b/Ege Zeitplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\010-IPA\IPA-Dokumentation\Tag1\IPA-Dok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egebo\Desktop\IPA-Dok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E7BB04-0802-4CDF-951D-D283EF7A9123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712833DD-6F7A-4214-B3E9-D2185F610CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB9C6447-36BB-4D67-BBCE-08BA330606A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
   <si>
     <t>Nr.</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Testkonzept</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>Analyse des bestehenden Source-Codes von HelpDeskZ.</t>
   </si>
   <si>
@@ -287,12 +284,6 @@
     <t>Konzept erstellen davor, danach</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>Auswertung</t>
   </si>
   <si>
@@ -309,6 +300,18 @@
   </si>
   <si>
     <t>Fazit</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -668,107 +671,113 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1107,7 +1116,7 @@
   <dimension ref="A1:AS67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E19"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,151 +1128,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="46" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="46" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="46" t="s">
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="46" t="s">
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="46" t="s">
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="46" t="s">
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="46" t="s">
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="46" t="s">
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="46" t="s">
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="43"/>
+      <c r="AK1" s="43"/>
+      <c r="AL1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="47"/>
-      <c r="AP1" s="46" t="s">
+      <c r="AM1" s="43"/>
+      <c r="AN1" s="43"/>
+      <c r="AO1" s="43"/>
+      <c r="AP1" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="AQ1" s="47"/>
-      <c r="AR1" s="47"/>
-      <c r="AS1" s="48"/>
+      <c r="AQ1" s="43"/>
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="44"/>
     </row>
     <row r="2" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="40" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="40" t="s">
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="40" t="s">
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="40" t="s">
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="40" t="s">
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="40" t="s">
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="40" t="s">
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="40" t="s">
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AI2" s="41"/>
-      <c r="AJ2" s="41"/>
-      <c r="AK2" s="41"/>
-      <c r="AL2" s="40" t="s">
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="AM2" s="41"/>
-      <c r="AN2" s="41"/>
-      <c r="AO2" s="41"/>
-      <c r="AP2" s="40" t="s">
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AQ2" s="41"/>
-      <c r="AR2" s="41"/>
-      <c r="AS2" s="42"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="38"/>
     </row>
     <row r="3" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1392,15 +1401,15 @@
       </c>
     </row>
     <row r="4" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
-      <c r="B4" s="33" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -1443,11 +1452,11 @@
       <c r="AS4" s="12"/>
     </row>
     <row r="5" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="50"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -1490,17 +1499,17 @@
       <c r="AS5" s="10"/>
     </row>
     <row r="6" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="31">
         <v>1</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1543,11 +1552,11 @@
       <c r="AS6" s="10"/>
     </row>
     <row r="7" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -1590,17 +1599,17 @@
       <c r="AS7" s="10"/>
     </row>
     <row r="8" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="31">
         <v>2</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1636,18 +1645,18 @@
       <c r="AL8" s="6"/>
       <c r="AM8" s="6"/>
       <c r="AN8" s="6"/>
-      <c r="AO8" s="12"/>
-      <c r="AP8" s="6"/>
+      <c r="AO8" s="58"/>
+      <c r="AP8" s="11"/>
       <c r="AQ8" s="6"/>
       <c r="AR8" s="6"/>
       <c r="AS8" s="10"/>
     </row>
     <row r="9" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1690,17 +1699,17 @@
       <c r="AS9" s="10"/>
     </row>
     <row r="10" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="31"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="31">
         <v>1</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="31">
         <v>1</v>
       </c>
       <c r="F10" s="11"/>
@@ -1745,11 +1754,11 @@
       <c r="AS10" s="10"/>
     </row>
     <row r="11" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="23"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
@@ -1792,19 +1801,19 @@
       <c r="AS11" s="22"/>
     </row>
     <row r="12" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="24">
+      <c r="C12" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="31">
         <v>1</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="31">
         <v>1</v>
       </c>
       <c r="F12" s="6"/>
@@ -1849,11 +1858,11 @@
       <c r="AS12" s="10"/>
     </row>
     <row r="13" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1896,17 +1905,17 @@
       <c r="AS13" s="10"/>
     </row>
     <row r="14" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
-      <c r="B14" s="33" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="31">
         <v>1</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="31">
         <v>1</v>
       </c>
       <c r="F14" s="6"/>
@@ -1951,11 +1960,11 @@
       <c r="AS14" s="10"/>
     </row>
     <row r="15" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="6"/>
       <c r="G15" s="13"/>
       <c r="H15" s="6"/>
@@ -1998,17 +2007,17 @@
       <c r="AS15" s="10"/>
     </row>
     <row r="16" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="33" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="24">
+      <c r="C16" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="31">
         <v>2</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="31">
         <v>2</v>
       </c>
       <c r="F16" s="6"/>
@@ -2053,11 +2062,11 @@
       <c r="AS16" s="10"/>
     </row>
     <row r="17" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="32"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -2100,19 +2109,19 @@
       <c r="AS17" s="10"/>
     </row>
     <row r="18" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="31">
         <v>4</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="31">
         <v>4.5</v>
       </c>
       <c r="F18" s="6"/>
@@ -2157,11 +2166,11 @@
       <c r="AS18" s="10"/>
     </row>
     <row r="19" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="31"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="13"/>
@@ -2204,17 +2213,17 @@
       <c r="AS19" s="10"/>
     </row>
     <row r="20" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="33" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="24">
+      <c r="C20" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="31">
         <v>2</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="31">
         <v>2</v>
       </c>
       <c r="F20" s="6"/>
@@ -2259,11 +2268,11 @@
       <c r="AS20" s="10"/>
     </row>
     <row r="21" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -2306,17 +2315,17 @@
       <c r="AS21" s="10"/>
     </row>
     <row r="22" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="33" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="24">
+      <c r="C22" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="31">
         <v>2</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -2359,11 +2368,11 @@
       <c r="AS22" s="10"/>
     </row>
     <row r="23" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -2406,17 +2415,17 @@
       <c r="AS23" s="10"/>
     </row>
     <row r="24" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="24">
+      <c r="A24" s="25"/>
+      <c r="B24" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="31">
         <v>2</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -2459,11 +2468,11 @@
       <c r="AS24" s="10"/>
     </row>
     <row r="25" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -2506,17 +2515,17 @@
       <c r="AS25" s="10"/>
     </row>
     <row r="26" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="28" t="s">
+      <c r="A26" s="25"/>
+      <c r="B26" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="31">
         <v>2</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -2559,11 +2568,11 @@
       <c r="AS26" s="10"/>
     </row>
     <row r="27" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="31"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -2606,14 +2615,14 @@
       <c r="AS27" s="10"/>
     </row>
     <row r="28" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="31"/>
-      <c r="B28" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="28" t="s">
+      <c r="A28" s="25"/>
+      <c r="B28" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="31">
         <v>2</v>
       </c>
       <c r="E28" s="15"/>
@@ -2659,10 +2668,10 @@
       <c r="AS28" s="10"/>
     </row>
     <row r="29" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="32"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="25"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="15"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2706,19 +2715,19 @@
       <c r="AS29" s="10"/>
     </row>
     <row r="30" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="24">
+      <c r="B30" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="31">
         <v>1</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -2761,11 +2770,11 @@
       <c r="AS30" s="10"/>
     </row>
     <row r="31" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="31"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -2808,17 +2817,17 @@
       <c r="AS31" s="10"/>
     </row>
     <row r="32" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="31"/>
-      <c r="B32" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="28" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="31">
         <v>1</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="31"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -2861,11 +2870,11 @@
       <c r="AS32" s="10"/>
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="32"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -2908,19 +2917,19 @@
       <c r="AS33" s="10"/>
     </row>
     <row r="34" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="24">
+      <c r="B34" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="31">
         <v>2</v>
       </c>
-      <c r="E34" s="24"/>
+      <c r="E34" s="31"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -2963,11 +2972,11 @@
       <c r="AS34" s="10"/>
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="31"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -3010,17 +3019,17 @@
       <c r="AS35" s="10"/>
     </row>
     <row r="36" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="31"/>
-      <c r="B36" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="24">
+      <c r="A36" s="25"/>
+      <c r="B36" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="31">
         <v>8</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="31"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -3063,11 +3072,11 @@
       <c r="AS36" s="10"/>
     </row>
     <row r="37" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="31"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -3110,17 +3119,17 @@
       <c r="AS37" s="10"/>
     </row>
     <row r="38" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="31"/>
-      <c r="B38" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="24">
+      <c r="A38" s="25"/>
+      <c r="B38" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="31">
         <v>8</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -3163,11 +3172,11 @@
       <c r="AS38" s="10"/>
     </row>
     <row r="39" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="31"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -3210,17 +3219,17 @@
       <c r="AS39" s="10"/>
     </row>
     <row r="40" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="31"/>
-      <c r="B40" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="24">
+      <c r="A40" s="25"/>
+      <c r="B40" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="31">
         <v>4</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="31"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -3263,11 +3272,11 @@
       <c r="AS40" s="10"/>
     </row>
     <row r="41" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="31"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -3310,17 +3319,17 @@
       <c r="AS41" s="10"/>
     </row>
     <row r="42" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="31"/>
-      <c r="B42" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="24">
+      <c r="A42" s="25"/>
+      <c r="B42" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="31">
         <v>4</v>
       </c>
-      <c r="E42" s="24"/>
+      <c r="E42" s="31"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -3363,11 +3372,11 @@
       <c r="AS42" s="10"/>
     </row>
     <row r="43" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="31"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -3410,19 +3419,19 @@
       <c r="AS43" s="10"/>
     </row>
     <row r="44" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D44" s="24">
+      <c r="D44" s="31">
         <v>2</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="31"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -3465,11 +3474,11 @@
       <c r="AS44" s="10"/>
     </row>
     <row r="45" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="31"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -3512,17 +3521,17 @@
       <c r="AS45" s="10"/>
     </row>
     <row r="46" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="31"/>
-      <c r="B46" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D46" s="24">
+      <c r="A46" s="25"/>
+      <c r="B46" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="31">
         <v>8</v>
       </c>
-      <c r="E46" s="24"/>
+      <c r="E46" s="31"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -3565,11 +3574,11 @@
       <c r="AS46" s="10"/>
     </row>
     <row r="47" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="32"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -3612,19 +3621,19 @@
       <c r="AS47" s="10"/>
     </row>
     <row r="48" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" s="24">
+      <c r="A48" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="31">
         <v>2</v>
       </c>
-      <c r="E48" s="24"/>
+      <c r="E48" s="31"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
@@ -3667,11 +3676,11 @@
       <c r="AS48" s="10"/>
     </row>
     <row r="49" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="56"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
@@ -3714,17 +3723,17 @@
       <c r="AS49" s="10"/>
     </row>
     <row r="50" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="56"/>
-      <c r="B50" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="D50" s="24">
+      <c r="A50" s="34"/>
+      <c r="B50" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="31">
         <v>2</v>
       </c>
-      <c r="E50" s="24"/>
+      <c r="E50" s="31"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -3767,11 +3776,11 @@
       <c r="AS50" s="10"/>
     </row>
     <row r="51" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="56"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
@@ -3814,17 +3823,17 @@
       <c r="AS51" s="10"/>
     </row>
     <row r="52" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="56"/>
-      <c r="B52" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="24">
+      <c r="A52" s="34"/>
+      <c r="B52" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="31">
         <v>2</v>
       </c>
-      <c r="E52" s="24"/>
+      <c r="E52" s="31"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
@@ -3867,11 +3876,11 @@
       <c r="AS52" s="10"/>
     </row>
     <row r="53" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="56"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
@@ -3914,17 +3923,17 @@
       <c r="AS53" s="10"/>
     </row>
     <row r="54" spans="1:45" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="56"/>
-      <c r="B54" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" s="24">
+      <c r="A54" s="34"/>
+      <c r="B54" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="31">
         <v>2</v>
       </c>
-      <c r="E54" s="24"/>
+      <c r="E54" s="31"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
@@ -3967,11 +3976,11 @@
       <c r="AS54" s="10"/>
     </row>
     <row r="55" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="56"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
@@ -4014,17 +4023,17 @@
       <c r="AS55" s="10"/>
     </row>
     <row r="56" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="56"/>
-      <c r="B56" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" s="24">
+      <c r="A56" s="34"/>
+      <c r="B56" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="31">
         <v>2</v>
       </c>
-      <c r="E56" s="24"/>
+      <c r="E56" s="31"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
@@ -4060,18 +4069,18 @@
       <c r="AL56" s="6"/>
       <c r="AM56" s="6"/>
       <c r="AN56" s="6"/>
-      <c r="AO56" s="10"/>
-      <c r="AP56" s="11"/>
+      <c r="AO56" s="12"/>
+      <c r="AP56" s="59"/>
       <c r="AQ56" s="6"/>
       <c r="AR56" s="6"/>
       <c r="AS56" s="10"/>
     </row>
     <row r="57" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="57"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
+      <c r="A57" s="35"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
@@ -4217,46 +4226,46 @@
         <v>80</v>
       </c>
       <c r="E60" s="7"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="38"/>
-      <c r="L60" s="38"/>
-      <c r="M60" s="38"/>
-      <c r="N60" s="37"/>
-      <c r="O60" s="38"/>
-      <c r="P60" s="38"/>
-      <c r="Q60" s="38"/>
-      <c r="R60" s="37"/>
-      <c r="S60" s="38"/>
-      <c r="T60" s="38"/>
-      <c r="U60" s="38"/>
-      <c r="V60" s="37"/>
-      <c r="W60" s="38"/>
-      <c r="X60" s="38"/>
-      <c r="Y60" s="38"/>
-      <c r="Z60" s="37"/>
-      <c r="AA60" s="38"/>
-      <c r="AB60" s="38"/>
-      <c r="AC60" s="38"/>
-      <c r="AD60" s="37"/>
-      <c r="AE60" s="38"/>
-      <c r="AF60" s="38"/>
-      <c r="AG60" s="38"/>
-      <c r="AH60" s="37"/>
-      <c r="AI60" s="38"/>
-      <c r="AJ60" s="38"/>
-      <c r="AK60" s="38"/>
-      <c r="AL60" s="37"/>
-      <c r="AM60" s="38"/>
-      <c r="AN60" s="38"/>
-      <c r="AO60" s="38"/>
-      <c r="AP60" s="37"/>
-      <c r="AQ60" s="38"/>
-      <c r="AR60" s="38"/>
-      <c r="AS60" s="39"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="51"/>
+      <c r="K60" s="52"/>
+      <c r="L60" s="52"/>
+      <c r="M60" s="52"/>
+      <c r="N60" s="51"/>
+      <c r="O60" s="52"/>
+      <c r="P60" s="52"/>
+      <c r="Q60" s="52"/>
+      <c r="R60" s="51"/>
+      <c r="S60" s="52"/>
+      <c r="T60" s="52"/>
+      <c r="U60" s="52"/>
+      <c r="V60" s="51"/>
+      <c r="W60" s="52"/>
+      <c r="X60" s="52"/>
+      <c r="Y60" s="52"/>
+      <c r="Z60" s="51"/>
+      <c r="AA60" s="52"/>
+      <c r="AB60" s="52"/>
+      <c r="AC60" s="52"/>
+      <c r="AD60" s="51"/>
+      <c r="AE60" s="52"/>
+      <c r="AF60" s="52"/>
+      <c r="AG60" s="52"/>
+      <c r="AH60" s="51"/>
+      <c r="AI60" s="52"/>
+      <c r="AJ60" s="52"/>
+      <c r="AK60" s="52"/>
+      <c r="AL60" s="51"/>
+      <c r="AM60" s="52"/>
+      <c r="AN60" s="52"/>
+      <c r="AO60" s="52"/>
+      <c r="AP60" s="51"/>
+      <c r="AQ60" s="52"/>
+      <c r="AR60" s="52"/>
+      <c r="AS60" s="53"/>
     </row>
     <row r="61" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
@@ -4264,46 +4273,46 @@
       <c r="C61" s="7"/>
       <c r="D61" s="4"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="38"/>
-      <c r="I61" s="38"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="38"/>
-      <c r="L61" s="38"/>
-      <c r="M61" s="38"/>
-      <c r="N61" s="37"/>
-      <c r="O61" s="38"/>
-      <c r="P61" s="38"/>
-      <c r="Q61" s="38"/>
-      <c r="R61" s="37"/>
-      <c r="S61" s="38"/>
-      <c r="T61" s="38"/>
-      <c r="U61" s="38"/>
-      <c r="V61" s="37"/>
-      <c r="W61" s="38"/>
-      <c r="X61" s="38"/>
-      <c r="Y61" s="38"/>
-      <c r="Z61" s="37"/>
-      <c r="AA61" s="38"/>
-      <c r="AB61" s="38"/>
-      <c r="AC61" s="38"/>
-      <c r="AD61" s="37"/>
-      <c r="AE61" s="38"/>
-      <c r="AF61" s="38"/>
-      <c r="AG61" s="38"/>
-      <c r="AH61" s="37"/>
-      <c r="AI61" s="38"/>
-      <c r="AJ61" s="38"/>
-      <c r="AK61" s="38"/>
-      <c r="AL61" s="37"/>
-      <c r="AM61" s="38"/>
-      <c r="AN61" s="38"/>
-      <c r="AO61" s="38"/>
-      <c r="AP61" s="37"/>
-      <c r="AQ61" s="38"/>
-      <c r="AR61" s="38"/>
-      <c r="AS61" s="39"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="51"/>
+      <c r="K61" s="52"/>
+      <c r="L61" s="52"/>
+      <c r="M61" s="52"/>
+      <c r="N61" s="51"/>
+      <c r="O61" s="52"/>
+      <c r="P61" s="52"/>
+      <c r="Q61" s="52"/>
+      <c r="R61" s="51"/>
+      <c r="S61" s="52"/>
+      <c r="T61" s="52"/>
+      <c r="U61" s="52"/>
+      <c r="V61" s="51"/>
+      <c r="W61" s="52"/>
+      <c r="X61" s="52"/>
+      <c r="Y61" s="52"/>
+      <c r="Z61" s="51"/>
+      <c r="AA61" s="52"/>
+      <c r="AB61" s="52"/>
+      <c r="AC61" s="52"/>
+      <c r="AD61" s="51"/>
+      <c r="AE61" s="52"/>
+      <c r="AF61" s="52"/>
+      <c r="AG61" s="52"/>
+      <c r="AH61" s="51"/>
+      <c r="AI61" s="52"/>
+      <c r="AJ61" s="52"/>
+      <c r="AK61" s="52"/>
+      <c r="AL61" s="51"/>
+      <c r="AM61" s="52"/>
+      <c r="AN61" s="52"/>
+      <c r="AO61" s="52"/>
+      <c r="AP61" s="51"/>
+      <c r="AQ61" s="52"/>
+      <c r="AR61" s="52"/>
+      <c r="AS61" s="53"/>
     </row>
     <row r="62" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
@@ -4313,46 +4322,46 @@
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="7"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="38"/>
-      <c r="I62" s="38"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="38"/>
-      <c r="L62" s="38"/>
-      <c r="M62" s="38"/>
-      <c r="N62" s="37"/>
-      <c r="O62" s="38"/>
-      <c r="P62" s="38"/>
-      <c r="Q62" s="38"/>
-      <c r="R62" s="37"/>
-      <c r="S62" s="38"/>
-      <c r="T62" s="38"/>
-      <c r="U62" s="38"/>
-      <c r="V62" s="37"/>
-      <c r="W62" s="38"/>
-      <c r="X62" s="38"/>
-      <c r="Y62" s="38"/>
-      <c r="Z62" s="37"/>
-      <c r="AA62" s="38"/>
-      <c r="AB62" s="38"/>
-      <c r="AC62" s="38"/>
-      <c r="AD62" s="37"/>
-      <c r="AE62" s="38"/>
-      <c r="AF62" s="38"/>
-      <c r="AG62" s="38"/>
-      <c r="AH62" s="37"/>
-      <c r="AI62" s="38"/>
-      <c r="AJ62" s="38"/>
-      <c r="AK62" s="38"/>
-      <c r="AL62" s="37"/>
-      <c r="AM62" s="38"/>
-      <c r="AN62" s="38"/>
-      <c r="AO62" s="38"/>
-      <c r="AP62" s="37"/>
-      <c r="AQ62" s="38"/>
-      <c r="AR62" s="38"/>
-      <c r="AS62" s="39"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="52"/>
+      <c r="M62" s="52"/>
+      <c r="N62" s="51"/>
+      <c r="O62" s="52"/>
+      <c r="P62" s="52"/>
+      <c r="Q62" s="52"/>
+      <c r="R62" s="51"/>
+      <c r="S62" s="52"/>
+      <c r="T62" s="52"/>
+      <c r="U62" s="52"/>
+      <c r="V62" s="51"/>
+      <c r="W62" s="52"/>
+      <c r="X62" s="52"/>
+      <c r="Y62" s="52"/>
+      <c r="Z62" s="51"/>
+      <c r="AA62" s="52"/>
+      <c r="AB62" s="52"/>
+      <c r="AC62" s="52"/>
+      <c r="AD62" s="51"/>
+      <c r="AE62" s="52"/>
+      <c r="AF62" s="52"/>
+      <c r="AG62" s="52"/>
+      <c r="AH62" s="51"/>
+      <c r="AI62" s="52"/>
+      <c r="AJ62" s="52"/>
+      <c r="AK62" s="52"/>
+      <c r="AL62" s="51"/>
+      <c r="AM62" s="52"/>
+      <c r="AN62" s="52"/>
+      <c r="AO62" s="52"/>
+      <c r="AP62" s="51"/>
+      <c r="AQ62" s="52"/>
+      <c r="AR62" s="52"/>
+      <c r="AS62" s="53"/>
     </row>
     <row r="63" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
@@ -4360,46 +4369,46 @@
       <c r="C63" s="3"/>
       <c r="D63" s="4"/>
       <c r="E63" s="7"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="38"/>
-      <c r="J63" s="37"/>
-      <c r="K63" s="38"/>
-      <c r="L63" s="38"/>
-      <c r="M63" s="38"/>
-      <c r="N63" s="37"/>
-      <c r="O63" s="38"/>
-      <c r="P63" s="38"/>
-      <c r="Q63" s="38"/>
-      <c r="R63" s="37"/>
-      <c r="S63" s="38"/>
-      <c r="T63" s="38"/>
-      <c r="U63" s="38"/>
-      <c r="V63" s="37"/>
-      <c r="W63" s="38"/>
-      <c r="X63" s="38"/>
-      <c r="Y63" s="38"/>
-      <c r="Z63" s="37"/>
-      <c r="AA63" s="38"/>
-      <c r="AB63" s="38"/>
-      <c r="AC63" s="38"/>
-      <c r="AD63" s="37"/>
-      <c r="AE63" s="38"/>
-      <c r="AF63" s="38"/>
-      <c r="AG63" s="38"/>
-      <c r="AH63" s="37"/>
-      <c r="AI63" s="38"/>
-      <c r="AJ63" s="38"/>
-      <c r="AK63" s="38"/>
-      <c r="AL63" s="37"/>
-      <c r="AM63" s="38"/>
-      <c r="AN63" s="38"/>
-      <c r="AO63" s="38"/>
-      <c r="AP63" s="37"/>
-      <c r="AQ63" s="38"/>
-      <c r="AR63" s="38"/>
-      <c r="AS63" s="39"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="51"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="52"/>
+      <c r="N63" s="51"/>
+      <c r="O63" s="52"/>
+      <c r="P63" s="52"/>
+      <c r="Q63" s="52"/>
+      <c r="R63" s="51"/>
+      <c r="S63" s="52"/>
+      <c r="T63" s="52"/>
+      <c r="U63" s="52"/>
+      <c r="V63" s="51"/>
+      <c r="W63" s="52"/>
+      <c r="X63" s="52"/>
+      <c r="Y63" s="52"/>
+      <c r="Z63" s="51"/>
+      <c r="AA63" s="52"/>
+      <c r="AB63" s="52"/>
+      <c r="AC63" s="52"/>
+      <c r="AD63" s="51"/>
+      <c r="AE63" s="52"/>
+      <c r="AF63" s="52"/>
+      <c r="AG63" s="52"/>
+      <c r="AH63" s="51"/>
+      <c r="AI63" s="52"/>
+      <c r="AJ63" s="52"/>
+      <c r="AK63" s="52"/>
+      <c r="AL63" s="51"/>
+      <c r="AM63" s="52"/>
+      <c r="AN63" s="52"/>
+      <c r="AO63" s="52"/>
+      <c r="AP63" s="51"/>
+      <c r="AQ63" s="52"/>
+      <c r="AR63" s="52"/>
+      <c r="AS63" s="53"/>
     </row>
     <row r="64" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
@@ -4407,46 +4416,46 @@
       <c r="C64" s="3"/>
       <c r="D64" s="4"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="38"/>
-      <c r="M64" s="38"/>
-      <c r="N64" s="37"/>
-      <c r="O64" s="38"/>
-      <c r="P64" s="38"/>
-      <c r="Q64" s="38"/>
-      <c r="R64" s="37"/>
-      <c r="S64" s="38"/>
-      <c r="T64" s="38"/>
-      <c r="U64" s="38"/>
-      <c r="V64" s="37"/>
-      <c r="W64" s="38"/>
-      <c r="X64" s="38"/>
-      <c r="Y64" s="38"/>
-      <c r="Z64" s="37"/>
-      <c r="AA64" s="38"/>
-      <c r="AB64" s="38"/>
-      <c r="AC64" s="38"/>
-      <c r="AD64" s="37"/>
-      <c r="AE64" s="38"/>
-      <c r="AF64" s="38"/>
-      <c r="AG64" s="38"/>
-      <c r="AH64" s="37"/>
-      <c r="AI64" s="38"/>
-      <c r="AJ64" s="38"/>
-      <c r="AK64" s="38"/>
-      <c r="AL64" s="37"/>
-      <c r="AM64" s="38"/>
-      <c r="AN64" s="38"/>
-      <c r="AO64" s="38"/>
-      <c r="AP64" s="37"/>
-      <c r="AQ64" s="38"/>
-      <c r="AR64" s="38"/>
-      <c r="AS64" s="39"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="52"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="51"/>
+      <c r="K64" s="52"/>
+      <c r="L64" s="52"/>
+      <c r="M64" s="52"/>
+      <c r="N64" s="51"/>
+      <c r="O64" s="52"/>
+      <c r="P64" s="52"/>
+      <c r="Q64" s="52"/>
+      <c r="R64" s="51"/>
+      <c r="S64" s="52"/>
+      <c r="T64" s="52"/>
+      <c r="U64" s="52"/>
+      <c r="V64" s="51"/>
+      <c r="W64" s="52"/>
+      <c r="X64" s="52"/>
+      <c r="Y64" s="52"/>
+      <c r="Z64" s="51"/>
+      <c r="AA64" s="52"/>
+      <c r="AB64" s="52"/>
+      <c r="AC64" s="52"/>
+      <c r="AD64" s="51"/>
+      <c r="AE64" s="52"/>
+      <c r="AF64" s="52"/>
+      <c r="AG64" s="52"/>
+      <c r="AH64" s="51"/>
+      <c r="AI64" s="52"/>
+      <c r="AJ64" s="52"/>
+      <c r="AK64" s="52"/>
+      <c r="AL64" s="51"/>
+      <c r="AM64" s="52"/>
+      <c r="AN64" s="52"/>
+      <c r="AO64" s="52"/>
+      <c r="AP64" s="51"/>
+      <c r="AQ64" s="52"/>
+      <c r="AR64" s="52"/>
+      <c r="AS64" s="53"/>
     </row>
     <row r="65" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
@@ -4454,46 +4463,46 @@
       <c r="C65" s="3"/>
       <c r="D65" s="4"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="38"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="38"/>
-      <c r="L65" s="38"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="37"/>
-      <c r="O65" s="38"/>
-      <c r="P65" s="38"/>
-      <c r="Q65" s="38"/>
-      <c r="R65" s="37"/>
-      <c r="S65" s="38"/>
-      <c r="T65" s="38"/>
-      <c r="U65" s="38"/>
-      <c r="V65" s="37"/>
-      <c r="W65" s="38"/>
-      <c r="X65" s="38"/>
-      <c r="Y65" s="38"/>
-      <c r="Z65" s="37"/>
-      <c r="AA65" s="38"/>
-      <c r="AB65" s="38"/>
-      <c r="AC65" s="38"/>
-      <c r="AD65" s="37"/>
-      <c r="AE65" s="38"/>
-      <c r="AF65" s="38"/>
-      <c r="AG65" s="38"/>
-      <c r="AH65" s="37"/>
-      <c r="AI65" s="38"/>
-      <c r="AJ65" s="38"/>
-      <c r="AK65" s="38"/>
-      <c r="AL65" s="37"/>
-      <c r="AM65" s="38"/>
-      <c r="AN65" s="38"/>
-      <c r="AO65" s="38"/>
-      <c r="AP65" s="37"/>
-      <c r="AQ65" s="38"/>
-      <c r="AR65" s="38"/>
-      <c r="AS65" s="39"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="51"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="52"/>
+      <c r="N65" s="51"/>
+      <c r="O65" s="52"/>
+      <c r="P65" s="52"/>
+      <c r="Q65" s="52"/>
+      <c r="R65" s="51"/>
+      <c r="S65" s="52"/>
+      <c r="T65" s="52"/>
+      <c r="U65" s="52"/>
+      <c r="V65" s="51"/>
+      <c r="W65" s="52"/>
+      <c r="X65" s="52"/>
+      <c r="Y65" s="52"/>
+      <c r="Z65" s="51"/>
+      <c r="AA65" s="52"/>
+      <c r="AB65" s="52"/>
+      <c r="AC65" s="52"/>
+      <c r="AD65" s="51"/>
+      <c r="AE65" s="52"/>
+      <c r="AF65" s="52"/>
+      <c r="AG65" s="52"/>
+      <c r="AH65" s="51"/>
+      <c r="AI65" s="52"/>
+      <c r="AJ65" s="52"/>
+      <c r="AK65" s="52"/>
+      <c r="AL65" s="51"/>
+      <c r="AM65" s="52"/>
+      <c r="AN65" s="52"/>
+      <c r="AO65" s="52"/>
+      <c r="AP65" s="51"/>
+      <c r="AQ65" s="52"/>
+      <c r="AR65" s="52"/>
+      <c r="AS65" s="53"/>
     </row>
     <row r="66" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
@@ -4501,70 +4510,212 @@
       <c r="C66" s="3"/>
       <c r="D66" s="4"/>
       <c r="E66" s="7"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="37"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="38"/>
-      <c r="M66" s="38"/>
-      <c r="N66" s="37"/>
-      <c r="O66" s="38"/>
-      <c r="P66" s="38"/>
-      <c r="Q66" s="38"/>
-      <c r="R66" s="37"/>
-      <c r="S66" s="38"/>
-      <c r="T66" s="38"/>
-      <c r="U66" s="38"/>
-      <c r="V66" s="37"/>
-      <c r="W66" s="38"/>
-      <c r="X66" s="38"/>
-      <c r="Y66" s="38"/>
-      <c r="Z66" s="37"/>
-      <c r="AA66" s="38"/>
-      <c r="AB66" s="38"/>
-      <c r="AC66" s="38"/>
-      <c r="AD66" s="37"/>
-      <c r="AE66" s="38"/>
-      <c r="AF66" s="38"/>
-      <c r="AG66" s="38"/>
-      <c r="AH66" s="37"/>
-      <c r="AI66" s="38"/>
-      <c r="AJ66" s="38"/>
-      <c r="AK66" s="38"/>
-      <c r="AL66" s="37"/>
-      <c r="AM66" s="38"/>
-      <c r="AN66" s="38"/>
-      <c r="AO66" s="38"/>
-      <c r="AP66" s="37"/>
-      <c r="AQ66" s="38"/>
-      <c r="AR66" s="38"/>
-      <c r="AS66" s="39"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="52"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="52"/>
+      <c r="L66" s="52"/>
+      <c r="M66" s="52"/>
+      <c r="N66" s="51"/>
+      <c r="O66" s="52"/>
+      <c r="P66" s="52"/>
+      <c r="Q66" s="52"/>
+      <c r="R66" s="51"/>
+      <c r="S66" s="52"/>
+      <c r="T66" s="52"/>
+      <c r="U66" s="52"/>
+      <c r="V66" s="51"/>
+      <c r="W66" s="52"/>
+      <c r="X66" s="52"/>
+      <c r="Y66" s="52"/>
+      <c r="Z66" s="51"/>
+      <c r="AA66" s="52"/>
+      <c r="AB66" s="52"/>
+      <c r="AC66" s="52"/>
+      <c r="AD66" s="51"/>
+      <c r="AE66" s="52"/>
+      <c r="AF66" s="52"/>
+      <c r="AG66" s="52"/>
+      <c r="AH66" s="51"/>
+      <c r="AI66" s="52"/>
+      <c r="AJ66" s="52"/>
+      <c r="AK66" s="52"/>
+      <c r="AL66" s="51"/>
+      <c r="AM66" s="52"/>
+      <c r="AN66" s="52"/>
+      <c r="AO66" s="52"/>
+      <c r="AP66" s="51"/>
+      <c r="AQ66" s="52"/>
+      <c r="AR66" s="52"/>
+      <c r="AS66" s="53"/>
     </row>
     <row r="67" spans="1:45" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="208">
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="AH62:AK62"/>
+    <mergeCell ref="AL62:AO62"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="AP66:AS66"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="AD65:AG65"/>
+    <mergeCell ref="AH65:AK65"/>
+    <mergeCell ref="AL65:AO65"/>
+    <mergeCell ref="AP65:AS65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="N66:Q66"/>
+    <mergeCell ref="R66:U66"/>
+    <mergeCell ref="V66:Y66"/>
+    <mergeCell ref="Z66:AC66"/>
+    <mergeCell ref="AD64:AG64"/>
+    <mergeCell ref="AD66:AG66"/>
+    <mergeCell ref="AH66:AK66"/>
+    <mergeCell ref="AL66:AO66"/>
+    <mergeCell ref="V65:Y65"/>
+    <mergeCell ref="Z65:AC65"/>
+    <mergeCell ref="AD63:AG63"/>
+    <mergeCell ref="AH63:AK63"/>
+    <mergeCell ref="AL63:AO63"/>
+    <mergeCell ref="AP64:AS64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="N65:Q65"/>
+    <mergeCell ref="R65:U65"/>
+    <mergeCell ref="AP63:AS63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="N64:Q64"/>
+    <mergeCell ref="R64:U64"/>
+    <mergeCell ref="V64:Y64"/>
+    <mergeCell ref="Z64:AC64"/>
+    <mergeCell ref="AH64:AK64"/>
+    <mergeCell ref="AL64:AO64"/>
+    <mergeCell ref="AP62:AS62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="N63:Q63"/>
+    <mergeCell ref="R63:U63"/>
+    <mergeCell ref="V63:Y63"/>
+    <mergeCell ref="Z63:AC63"/>
+    <mergeCell ref="AP61:AS61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="N62:Q62"/>
+    <mergeCell ref="R62:U62"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="Z62:AC62"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="N61:Q61"/>
+    <mergeCell ref="R61:U61"/>
+    <mergeCell ref="V61:Y61"/>
+    <mergeCell ref="Z61:AC61"/>
+    <mergeCell ref="AD61:AG61"/>
+    <mergeCell ref="AH61:AK61"/>
+    <mergeCell ref="AL61:AO61"/>
+    <mergeCell ref="AD62:AG62"/>
+    <mergeCell ref="AP60:AS60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="R60:U60"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="V60:Y60"/>
+    <mergeCell ref="Z60:AC60"/>
+    <mergeCell ref="AD60:AG60"/>
+    <mergeCell ref="AH60:AK60"/>
+    <mergeCell ref="AL60:AO60"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="B56:B57"/>
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="D56:D57"/>
@@ -4589,172 +4740,30 @@
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A34:A43"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="AP60:AS60"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="N60:Q60"/>
-    <mergeCell ref="R60:U60"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="V60:Y60"/>
-    <mergeCell ref="Z60:AC60"/>
-    <mergeCell ref="AD60:AG60"/>
-    <mergeCell ref="AH60:AK60"/>
-    <mergeCell ref="AL60:AO60"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="AP62:AS62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="N63:Q63"/>
-    <mergeCell ref="R63:U63"/>
-    <mergeCell ref="V63:Y63"/>
-    <mergeCell ref="Z63:AC63"/>
-    <mergeCell ref="AP61:AS61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="N62:Q62"/>
-    <mergeCell ref="R62:U62"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="Z62:AC62"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="N61:Q61"/>
-    <mergeCell ref="R61:U61"/>
-    <mergeCell ref="V61:Y61"/>
-    <mergeCell ref="Z61:AC61"/>
-    <mergeCell ref="AD61:AG61"/>
-    <mergeCell ref="AH61:AK61"/>
-    <mergeCell ref="AL61:AO61"/>
-    <mergeCell ref="AD62:AG62"/>
-    <mergeCell ref="Z65:AC65"/>
-    <mergeCell ref="AD63:AG63"/>
-    <mergeCell ref="AH63:AK63"/>
-    <mergeCell ref="AL63:AO63"/>
-    <mergeCell ref="AP64:AS64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="J65:M65"/>
-    <mergeCell ref="N65:Q65"/>
-    <mergeCell ref="R65:U65"/>
-    <mergeCell ref="AP63:AS63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="N64:Q64"/>
-    <mergeCell ref="R64:U64"/>
-    <mergeCell ref="V64:Y64"/>
-    <mergeCell ref="Z64:AC64"/>
-    <mergeCell ref="AH64:AK64"/>
-    <mergeCell ref="AL64:AO64"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B52:B53"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="AP66:AS66"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="AD65:AG65"/>
-    <mergeCell ref="AH65:AK65"/>
-    <mergeCell ref="AL65:AO65"/>
-    <mergeCell ref="AP65:AS65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="N66:Q66"/>
-    <mergeCell ref="R66:U66"/>
-    <mergeCell ref="V66:Y66"/>
-    <mergeCell ref="Z66:AC66"/>
-    <mergeCell ref="AD64:AG64"/>
-    <mergeCell ref="AD66:AG66"/>
-    <mergeCell ref="AH66:AK66"/>
-    <mergeCell ref="AL66:AO66"/>
-    <mergeCell ref="V65:Y65"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="AH62:AK62"/>
-    <mergeCell ref="AL62:AO62"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
inital commit day 2, for uploading an uml diagram from draw.io
</commit_message>
<xml_diff>
--- a/Ege Zeitplan.xlsx
+++ b/Ege Zeitplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\010-IPA\IPA-Dokumentation\Tag1\IPA-Dok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egebo\Desktop\IPA-Dok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E7BB04-0802-4CDF-951D-D283EF7A9123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712833DD-6F7A-4214-B3E9-D2185F610CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB9C6447-36BB-4D67-BBCE-08BA330606A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
   <si>
     <t>Nr.</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Testkonzept</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>Analyse des bestehenden Source-Codes von HelpDeskZ.</t>
   </si>
   <si>
@@ -287,12 +284,6 @@
     <t>Konzept erstellen davor, danach</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>Auswertung</t>
   </si>
   <si>
@@ -309,6 +300,18 @@
   </si>
   <si>
     <t>Fazit</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -668,107 +671,113 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1107,7 +1116,7 @@
   <dimension ref="A1:AS67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E19"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,151 +1128,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="46" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="46" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="46" t="s">
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="46" t="s">
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="46" t="s">
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="46" t="s">
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="46" t="s">
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="46" t="s">
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="46" t="s">
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="43"/>
+      <c r="AK1" s="43"/>
+      <c r="AL1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="47"/>
-      <c r="AP1" s="46" t="s">
+      <c r="AM1" s="43"/>
+      <c r="AN1" s="43"/>
+      <c r="AO1" s="43"/>
+      <c r="AP1" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="AQ1" s="47"/>
-      <c r="AR1" s="47"/>
-      <c r="AS1" s="48"/>
+      <c r="AQ1" s="43"/>
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="44"/>
     </row>
     <row r="2" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="40" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="40" t="s">
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="40" t="s">
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="40" t="s">
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="40" t="s">
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="40" t="s">
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="40" t="s">
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="40" t="s">
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AI2" s="41"/>
-      <c r="AJ2" s="41"/>
-      <c r="AK2" s="41"/>
-      <c r="AL2" s="40" t="s">
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="AM2" s="41"/>
-      <c r="AN2" s="41"/>
-      <c r="AO2" s="41"/>
-      <c r="AP2" s="40" t="s">
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AQ2" s="41"/>
-      <c r="AR2" s="41"/>
-      <c r="AS2" s="42"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="38"/>
     </row>
     <row r="3" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1392,15 +1401,15 @@
       </c>
     </row>
     <row r="4" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
-      <c r="B4" s="33" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -1443,11 +1452,11 @@
       <c r="AS4" s="12"/>
     </row>
     <row r="5" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="50"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -1490,17 +1499,17 @@
       <c r="AS5" s="10"/>
     </row>
     <row r="6" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="31">
         <v>1</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1543,11 +1552,11 @@
       <c r="AS6" s="10"/>
     </row>
     <row r="7" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -1590,17 +1599,17 @@
       <c r="AS7" s="10"/>
     </row>
     <row r="8" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="31">
         <v>2</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1636,18 +1645,18 @@
       <c r="AL8" s="6"/>
       <c r="AM8" s="6"/>
       <c r="AN8" s="6"/>
-      <c r="AO8" s="12"/>
-      <c r="AP8" s="6"/>
+      <c r="AO8" s="58"/>
+      <c r="AP8" s="11"/>
       <c r="AQ8" s="6"/>
       <c r="AR8" s="6"/>
       <c r="AS8" s="10"/>
     </row>
     <row r="9" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1690,17 +1699,17 @@
       <c r="AS9" s="10"/>
     </row>
     <row r="10" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="31"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="31">
         <v>1</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="31">
         <v>1</v>
       </c>
       <c r="F10" s="11"/>
@@ -1745,11 +1754,11 @@
       <c r="AS10" s="10"/>
     </row>
     <row r="11" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="23"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
@@ -1792,19 +1801,19 @@
       <c r="AS11" s="22"/>
     </row>
     <row r="12" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="24">
+      <c r="C12" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="31">
         <v>1</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="31">
         <v>1</v>
       </c>
       <c r="F12" s="6"/>
@@ -1849,11 +1858,11 @@
       <c r="AS12" s="10"/>
     </row>
     <row r="13" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1896,17 +1905,17 @@
       <c r="AS13" s="10"/>
     </row>
     <row r="14" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
-      <c r="B14" s="33" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="31">
         <v>1</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="31">
         <v>1</v>
       </c>
       <c r="F14" s="6"/>
@@ -1951,11 +1960,11 @@
       <c r="AS14" s="10"/>
     </row>
     <row r="15" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="6"/>
       <c r="G15" s="13"/>
       <c r="H15" s="6"/>
@@ -1998,17 +2007,17 @@
       <c r="AS15" s="10"/>
     </row>
     <row r="16" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="33" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="24">
+      <c r="C16" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="31">
         <v>2</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="31">
         <v>2</v>
       </c>
       <c r="F16" s="6"/>
@@ -2053,11 +2062,11 @@
       <c r="AS16" s="10"/>
     </row>
     <row r="17" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="32"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -2100,19 +2109,19 @@
       <c r="AS17" s="10"/>
     </row>
     <row r="18" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="31">
         <v>4</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="31">
         <v>4.5</v>
       </c>
       <c r="F18" s="6"/>
@@ -2157,11 +2166,11 @@
       <c r="AS18" s="10"/>
     </row>
     <row r="19" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="31"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="13"/>
@@ -2204,17 +2213,17 @@
       <c r="AS19" s="10"/>
     </row>
     <row r="20" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="33" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="24">
+      <c r="C20" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="31">
         <v>2</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="31">
         <v>2</v>
       </c>
       <c r="F20" s="6"/>
@@ -2259,11 +2268,11 @@
       <c r="AS20" s="10"/>
     </row>
     <row r="21" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -2306,17 +2315,17 @@
       <c r="AS21" s="10"/>
     </row>
     <row r="22" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="33" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="24">
+      <c r="C22" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="31">
         <v>2</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -2359,11 +2368,11 @@
       <c r="AS22" s="10"/>
     </row>
     <row r="23" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -2406,17 +2415,17 @@
       <c r="AS23" s="10"/>
     </row>
     <row r="24" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="24">
+      <c r="A24" s="25"/>
+      <c r="B24" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="31">
         <v>2</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -2459,11 +2468,11 @@
       <c r="AS24" s="10"/>
     </row>
     <row r="25" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -2506,17 +2515,17 @@
       <c r="AS25" s="10"/>
     </row>
     <row r="26" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="28" t="s">
+      <c r="A26" s="25"/>
+      <c r="B26" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="31">
         <v>2</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -2559,11 +2568,11 @@
       <c r="AS26" s="10"/>
     </row>
     <row r="27" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="31"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -2606,14 +2615,14 @@
       <c r="AS27" s="10"/>
     </row>
     <row r="28" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="31"/>
-      <c r="B28" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="28" t="s">
+      <c r="A28" s="25"/>
+      <c r="B28" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="31">
         <v>2</v>
       </c>
       <c r="E28" s="15"/>
@@ -2659,10 +2668,10 @@
       <c r="AS28" s="10"/>
     </row>
     <row r="29" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="32"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="25"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="15"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2706,19 +2715,19 @@
       <c r="AS29" s="10"/>
     </row>
     <row r="30" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="24">
+      <c r="B30" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="31">
         <v>1</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -2761,11 +2770,11 @@
       <c r="AS30" s="10"/>
     </row>
     <row r="31" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="31"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -2808,17 +2817,17 @@
       <c r="AS31" s="10"/>
     </row>
     <row r="32" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="31"/>
-      <c r="B32" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="28" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="31">
         <v>1</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="31"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -2861,11 +2870,11 @@
       <c r="AS32" s="10"/>
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="32"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -2908,19 +2917,19 @@
       <c r="AS33" s="10"/>
     </row>
     <row r="34" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="24">
+      <c r="B34" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="31">
         <v>2</v>
       </c>
-      <c r="E34" s="24"/>
+      <c r="E34" s="31"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -2963,11 +2972,11 @@
       <c r="AS34" s="10"/>
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="31"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -3010,17 +3019,17 @@
       <c r="AS35" s="10"/>
     </row>
     <row r="36" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="31"/>
-      <c r="B36" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="24">
+      <c r="A36" s="25"/>
+      <c r="B36" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="31">
         <v>8</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="31"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -3063,11 +3072,11 @@
       <c r="AS36" s="10"/>
     </row>
     <row r="37" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="31"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -3110,17 +3119,17 @@
       <c r="AS37" s="10"/>
     </row>
     <row r="38" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="31"/>
-      <c r="B38" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="24">
+      <c r="A38" s="25"/>
+      <c r="B38" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="31">
         <v>8</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -3163,11 +3172,11 @@
       <c r="AS38" s="10"/>
     </row>
     <row r="39" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="31"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -3210,17 +3219,17 @@
       <c r="AS39" s="10"/>
     </row>
     <row r="40" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="31"/>
-      <c r="B40" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="24">
+      <c r="A40" s="25"/>
+      <c r="B40" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="31">
         <v>4</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="31"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -3263,11 +3272,11 @@
       <c r="AS40" s="10"/>
     </row>
     <row r="41" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="31"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -3310,17 +3319,17 @@
       <c r="AS41" s="10"/>
     </row>
     <row r="42" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="31"/>
-      <c r="B42" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="24">
+      <c r="A42" s="25"/>
+      <c r="B42" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="31">
         <v>4</v>
       </c>
-      <c r="E42" s="24"/>
+      <c r="E42" s="31"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -3363,11 +3372,11 @@
       <c r="AS42" s="10"/>
     </row>
     <row r="43" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="31"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -3410,19 +3419,19 @@
       <c r="AS43" s="10"/>
     </row>
     <row r="44" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D44" s="24">
+      <c r="D44" s="31">
         <v>2</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="31"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -3465,11 +3474,11 @@
       <c r="AS44" s="10"/>
     </row>
     <row r="45" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="31"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -3512,17 +3521,17 @@
       <c r="AS45" s="10"/>
     </row>
     <row r="46" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="31"/>
-      <c r="B46" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D46" s="24">
+      <c r="A46" s="25"/>
+      <c r="B46" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="31">
         <v>8</v>
       </c>
-      <c r="E46" s="24"/>
+      <c r="E46" s="31"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -3565,11 +3574,11 @@
       <c r="AS46" s="10"/>
     </row>
     <row r="47" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="32"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -3612,19 +3621,19 @@
       <c r="AS47" s="10"/>
     </row>
     <row r="48" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" s="24">
+      <c r="A48" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="31">
         <v>2</v>
       </c>
-      <c r="E48" s="24"/>
+      <c r="E48" s="31"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
@@ -3667,11 +3676,11 @@
       <c r="AS48" s="10"/>
     </row>
     <row r="49" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="56"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
@@ -3714,17 +3723,17 @@
       <c r="AS49" s="10"/>
     </row>
     <row r="50" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="56"/>
-      <c r="B50" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="D50" s="24">
+      <c r="A50" s="34"/>
+      <c r="B50" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="31">
         <v>2</v>
       </c>
-      <c r="E50" s="24"/>
+      <c r="E50" s="31"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -3767,11 +3776,11 @@
       <c r="AS50" s="10"/>
     </row>
     <row r="51" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="56"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
@@ -3814,17 +3823,17 @@
       <c r="AS51" s="10"/>
     </row>
     <row r="52" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="56"/>
-      <c r="B52" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="24">
+      <c r="A52" s="34"/>
+      <c r="B52" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="31">
         <v>2</v>
       </c>
-      <c r="E52" s="24"/>
+      <c r="E52" s="31"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
@@ -3867,11 +3876,11 @@
       <c r="AS52" s="10"/>
     </row>
     <row r="53" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="56"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
@@ -3914,17 +3923,17 @@
       <c r="AS53" s="10"/>
     </row>
     <row r="54" spans="1:45" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="56"/>
-      <c r="B54" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" s="24">
+      <c r="A54" s="34"/>
+      <c r="B54" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="31">
         <v>2</v>
       </c>
-      <c r="E54" s="24"/>
+      <c r="E54" s="31"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
@@ -3967,11 +3976,11 @@
       <c r="AS54" s="10"/>
     </row>
     <row r="55" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="56"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
@@ -4014,17 +4023,17 @@
       <c r="AS55" s="10"/>
     </row>
     <row r="56" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="56"/>
-      <c r="B56" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" s="24">
+      <c r="A56" s="34"/>
+      <c r="B56" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="31">
         <v>2</v>
       </c>
-      <c r="E56" s="24"/>
+      <c r="E56" s="31"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
@@ -4060,18 +4069,18 @@
       <c r="AL56" s="6"/>
       <c r="AM56" s="6"/>
       <c r="AN56" s="6"/>
-      <c r="AO56" s="10"/>
-      <c r="AP56" s="11"/>
+      <c r="AO56" s="12"/>
+      <c r="AP56" s="59"/>
       <c r="AQ56" s="6"/>
       <c r="AR56" s="6"/>
       <c r="AS56" s="10"/>
     </row>
     <row r="57" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="57"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
+      <c r="A57" s="35"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
@@ -4217,46 +4226,46 @@
         <v>80</v>
       </c>
       <c r="E60" s="7"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="38"/>
-      <c r="L60" s="38"/>
-      <c r="M60" s="38"/>
-      <c r="N60" s="37"/>
-      <c r="O60" s="38"/>
-      <c r="P60" s="38"/>
-      <c r="Q60" s="38"/>
-      <c r="R60" s="37"/>
-      <c r="S60" s="38"/>
-      <c r="T60" s="38"/>
-      <c r="U60" s="38"/>
-      <c r="V60" s="37"/>
-      <c r="W60" s="38"/>
-      <c r="X60" s="38"/>
-      <c r="Y60" s="38"/>
-      <c r="Z60" s="37"/>
-      <c r="AA60" s="38"/>
-      <c r="AB60" s="38"/>
-      <c r="AC60" s="38"/>
-      <c r="AD60" s="37"/>
-      <c r="AE60" s="38"/>
-      <c r="AF60" s="38"/>
-      <c r="AG60" s="38"/>
-      <c r="AH60" s="37"/>
-      <c r="AI60" s="38"/>
-      <c r="AJ60" s="38"/>
-      <c r="AK60" s="38"/>
-      <c r="AL60" s="37"/>
-      <c r="AM60" s="38"/>
-      <c r="AN60" s="38"/>
-      <c r="AO60" s="38"/>
-      <c r="AP60" s="37"/>
-      <c r="AQ60" s="38"/>
-      <c r="AR60" s="38"/>
-      <c r="AS60" s="39"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="51"/>
+      <c r="K60" s="52"/>
+      <c r="L60" s="52"/>
+      <c r="M60" s="52"/>
+      <c r="N60" s="51"/>
+      <c r="O60" s="52"/>
+      <c r="P60" s="52"/>
+      <c r="Q60" s="52"/>
+      <c r="R60" s="51"/>
+      <c r="S60" s="52"/>
+      <c r="T60" s="52"/>
+      <c r="U60" s="52"/>
+      <c r="V60" s="51"/>
+      <c r="W60" s="52"/>
+      <c r="X60" s="52"/>
+      <c r="Y60" s="52"/>
+      <c r="Z60" s="51"/>
+      <c r="AA60" s="52"/>
+      <c r="AB60" s="52"/>
+      <c r="AC60" s="52"/>
+      <c r="AD60" s="51"/>
+      <c r="AE60" s="52"/>
+      <c r="AF60" s="52"/>
+      <c r="AG60" s="52"/>
+      <c r="AH60" s="51"/>
+      <c r="AI60" s="52"/>
+      <c r="AJ60" s="52"/>
+      <c r="AK60" s="52"/>
+      <c r="AL60" s="51"/>
+      <c r="AM60" s="52"/>
+      <c r="AN60" s="52"/>
+      <c r="AO60" s="52"/>
+      <c r="AP60" s="51"/>
+      <c r="AQ60" s="52"/>
+      <c r="AR60" s="52"/>
+      <c r="AS60" s="53"/>
     </row>
     <row r="61" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
@@ -4264,46 +4273,46 @@
       <c r="C61" s="7"/>
       <c r="D61" s="4"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="38"/>
-      <c r="I61" s="38"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="38"/>
-      <c r="L61" s="38"/>
-      <c r="M61" s="38"/>
-      <c r="N61" s="37"/>
-      <c r="O61" s="38"/>
-      <c r="P61" s="38"/>
-      <c r="Q61" s="38"/>
-      <c r="R61" s="37"/>
-      <c r="S61" s="38"/>
-      <c r="T61" s="38"/>
-      <c r="U61" s="38"/>
-      <c r="V61" s="37"/>
-      <c r="W61" s="38"/>
-      <c r="X61" s="38"/>
-      <c r="Y61" s="38"/>
-      <c r="Z61" s="37"/>
-      <c r="AA61" s="38"/>
-      <c r="AB61" s="38"/>
-      <c r="AC61" s="38"/>
-      <c r="AD61" s="37"/>
-      <c r="AE61" s="38"/>
-      <c r="AF61" s="38"/>
-      <c r="AG61" s="38"/>
-      <c r="AH61" s="37"/>
-      <c r="AI61" s="38"/>
-      <c r="AJ61" s="38"/>
-      <c r="AK61" s="38"/>
-      <c r="AL61" s="37"/>
-      <c r="AM61" s="38"/>
-      <c r="AN61" s="38"/>
-      <c r="AO61" s="38"/>
-      <c r="AP61" s="37"/>
-      <c r="AQ61" s="38"/>
-      <c r="AR61" s="38"/>
-      <c r="AS61" s="39"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="51"/>
+      <c r="K61" s="52"/>
+      <c r="L61" s="52"/>
+      <c r="M61" s="52"/>
+      <c r="N61" s="51"/>
+      <c r="O61" s="52"/>
+      <c r="P61" s="52"/>
+      <c r="Q61" s="52"/>
+      <c r="R61" s="51"/>
+      <c r="S61" s="52"/>
+      <c r="T61" s="52"/>
+      <c r="U61" s="52"/>
+      <c r="V61" s="51"/>
+      <c r="W61" s="52"/>
+      <c r="X61" s="52"/>
+      <c r="Y61" s="52"/>
+      <c r="Z61" s="51"/>
+      <c r="AA61" s="52"/>
+      <c r="AB61" s="52"/>
+      <c r="AC61" s="52"/>
+      <c r="AD61" s="51"/>
+      <c r="AE61" s="52"/>
+      <c r="AF61" s="52"/>
+      <c r="AG61" s="52"/>
+      <c r="AH61" s="51"/>
+      <c r="AI61" s="52"/>
+      <c r="AJ61" s="52"/>
+      <c r="AK61" s="52"/>
+      <c r="AL61" s="51"/>
+      <c r="AM61" s="52"/>
+      <c r="AN61" s="52"/>
+      <c r="AO61" s="52"/>
+      <c r="AP61" s="51"/>
+      <c r="AQ61" s="52"/>
+      <c r="AR61" s="52"/>
+      <c r="AS61" s="53"/>
     </row>
     <row r="62" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
@@ -4313,46 +4322,46 @@
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="7"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="38"/>
-      <c r="I62" s="38"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="38"/>
-      <c r="L62" s="38"/>
-      <c r="M62" s="38"/>
-      <c r="N62" s="37"/>
-      <c r="O62" s="38"/>
-      <c r="P62" s="38"/>
-      <c r="Q62" s="38"/>
-      <c r="R62" s="37"/>
-      <c r="S62" s="38"/>
-      <c r="T62" s="38"/>
-      <c r="U62" s="38"/>
-      <c r="V62" s="37"/>
-      <c r="W62" s="38"/>
-      <c r="X62" s="38"/>
-      <c r="Y62" s="38"/>
-      <c r="Z62" s="37"/>
-      <c r="AA62" s="38"/>
-      <c r="AB62" s="38"/>
-      <c r="AC62" s="38"/>
-      <c r="AD62" s="37"/>
-      <c r="AE62" s="38"/>
-      <c r="AF62" s="38"/>
-      <c r="AG62" s="38"/>
-      <c r="AH62" s="37"/>
-      <c r="AI62" s="38"/>
-      <c r="AJ62" s="38"/>
-      <c r="AK62" s="38"/>
-      <c r="AL62" s="37"/>
-      <c r="AM62" s="38"/>
-      <c r="AN62" s="38"/>
-      <c r="AO62" s="38"/>
-      <c r="AP62" s="37"/>
-      <c r="AQ62" s="38"/>
-      <c r="AR62" s="38"/>
-      <c r="AS62" s="39"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="52"/>
+      <c r="M62" s="52"/>
+      <c r="N62" s="51"/>
+      <c r="O62" s="52"/>
+      <c r="P62" s="52"/>
+      <c r="Q62" s="52"/>
+      <c r="R62" s="51"/>
+      <c r="S62" s="52"/>
+      <c r="T62" s="52"/>
+      <c r="U62" s="52"/>
+      <c r="V62" s="51"/>
+      <c r="W62" s="52"/>
+      <c r="X62" s="52"/>
+      <c r="Y62" s="52"/>
+      <c r="Z62" s="51"/>
+      <c r="AA62" s="52"/>
+      <c r="AB62" s="52"/>
+      <c r="AC62" s="52"/>
+      <c r="AD62" s="51"/>
+      <c r="AE62" s="52"/>
+      <c r="AF62" s="52"/>
+      <c r="AG62" s="52"/>
+      <c r="AH62" s="51"/>
+      <c r="AI62" s="52"/>
+      <c r="AJ62" s="52"/>
+      <c r="AK62" s="52"/>
+      <c r="AL62" s="51"/>
+      <c r="AM62" s="52"/>
+      <c r="AN62" s="52"/>
+      <c r="AO62" s="52"/>
+      <c r="AP62" s="51"/>
+      <c r="AQ62" s="52"/>
+      <c r="AR62" s="52"/>
+      <c r="AS62" s="53"/>
     </row>
     <row r="63" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
@@ -4360,46 +4369,46 @@
       <c r="C63" s="3"/>
       <c r="D63" s="4"/>
       <c r="E63" s="7"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="38"/>
-      <c r="J63" s="37"/>
-      <c r="K63" s="38"/>
-      <c r="L63" s="38"/>
-      <c r="M63" s="38"/>
-      <c r="N63" s="37"/>
-      <c r="O63" s="38"/>
-      <c r="P63" s="38"/>
-      <c r="Q63" s="38"/>
-      <c r="R63" s="37"/>
-      <c r="S63" s="38"/>
-      <c r="T63" s="38"/>
-      <c r="U63" s="38"/>
-      <c r="V63" s="37"/>
-      <c r="W63" s="38"/>
-      <c r="X63" s="38"/>
-      <c r="Y63" s="38"/>
-      <c r="Z63" s="37"/>
-      <c r="AA63" s="38"/>
-      <c r="AB63" s="38"/>
-      <c r="AC63" s="38"/>
-      <c r="AD63" s="37"/>
-      <c r="AE63" s="38"/>
-      <c r="AF63" s="38"/>
-      <c r="AG63" s="38"/>
-      <c r="AH63" s="37"/>
-      <c r="AI63" s="38"/>
-      <c r="AJ63" s="38"/>
-      <c r="AK63" s="38"/>
-      <c r="AL63" s="37"/>
-      <c r="AM63" s="38"/>
-      <c r="AN63" s="38"/>
-      <c r="AO63" s="38"/>
-      <c r="AP63" s="37"/>
-      <c r="AQ63" s="38"/>
-      <c r="AR63" s="38"/>
-      <c r="AS63" s="39"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="51"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="52"/>
+      <c r="N63" s="51"/>
+      <c r="O63" s="52"/>
+      <c r="P63" s="52"/>
+      <c r="Q63" s="52"/>
+      <c r="R63" s="51"/>
+      <c r="S63" s="52"/>
+      <c r="T63" s="52"/>
+      <c r="U63" s="52"/>
+      <c r="V63" s="51"/>
+      <c r="W63" s="52"/>
+      <c r="X63" s="52"/>
+      <c r="Y63" s="52"/>
+      <c r="Z63" s="51"/>
+      <c r="AA63" s="52"/>
+      <c r="AB63" s="52"/>
+      <c r="AC63" s="52"/>
+      <c r="AD63" s="51"/>
+      <c r="AE63" s="52"/>
+      <c r="AF63" s="52"/>
+      <c r="AG63" s="52"/>
+      <c r="AH63" s="51"/>
+      <c r="AI63" s="52"/>
+      <c r="AJ63" s="52"/>
+      <c r="AK63" s="52"/>
+      <c r="AL63" s="51"/>
+      <c r="AM63" s="52"/>
+      <c r="AN63" s="52"/>
+      <c r="AO63" s="52"/>
+      <c r="AP63" s="51"/>
+      <c r="AQ63" s="52"/>
+      <c r="AR63" s="52"/>
+      <c r="AS63" s="53"/>
     </row>
     <row r="64" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
@@ -4407,46 +4416,46 @@
       <c r="C64" s="3"/>
       <c r="D64" s="4"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="38"/>
-      <c r="M64" s="38"/>
-      <c r="N64" s="37"/>
-      <c r="O64" s="38"/>
-      <c r="P64" s="38"/>
-      <c r="Q64" s="38"/>
-      <c r="R64" s="37"/>
-      <c r="S64" s="38"/>
-      <c r="T64" s="38"/>
-      <c r="U64" s="38"/>
-      <c r="V64" s="37"/>
-      <c r="W64" s="38"/>
-      <c r="X64" s="38"/>
-      <c r="Y64" s="38"/>
-      <c r="Z64" s="37"/>
-      <c r="AA64" s="38"/>
-      <c r="AB64" s="38"/>
-      <c r="AC64" s="38"/>
-      <c r="AD64" s="37"/>
-      <c r="AE64" s="38"/>
-      <c r="AF64" s="38"/>
-      <c r="AG64" s="38"/>
-      <c r="AH64" s="37"/>
-      <c r="AI64" s="38"/>
-      <c r="AJ64" s="38"/>
-      <c r="AK64" s="38"/>
-      <c r="AL64" s="37"/>
-      <c r="AM64" s="38"/>
-      <c r="AN64" s="38"/>
-      <c r="AO64" s="38"/>
-      <c r="AP64" s="37"/>
-      <c r="AQ64" s="38"/>
-      <c r="AR64" s="38"/>
-      <c r="AS64" s="39"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="52"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="51"/>
+      <c r="K64" s="52"/>
+      <c r="L64" s="52"/>
+      <c r="M64" s="52"/>
+      <c r="N64" s="51"/>
+      <c r="O64" s="52"/>
+      <c r="P64" s="52"/>
+      <c r="Q64" s="52"/>
+      <c r="R64" s="51"/>
+      <c r="S64" s="52"/>
+      <c r="T64" s="52"/>
+      <c r="U64" s="52"/>
+      <c r="V64" s="51"/>
+      <c r="W64" s="52"/>
+      <c r="X64" s="52"/>
+      <c r="Y64" s="52"/>
+      <c r="Z64" s="51"/>
+      <c r="AA64" s="52"/>
+      <c r="AB64" s="52"/>
+      <c r="AC64" s="52"/>
+      <c r="AD64" s="51"/>
+      <c r="AE64" s="52"/>
+      <c r="AF64" s="52"/>
+      <c r="AG64" s="52"/>
+      <c r="AH64" s="51"/>
+      <c r="AI64" s="52"/>
+      <c r="AJ64" s="52"/>
+      <c r="AK64" s="52"/>
+      <c r="AL64" s="51"/>
+      <c r="AM64" s="52"/>
+      <c r="AN64" s="52"/>
+      <c r="AO64" s="52"/>
+      <c r="AP64" s="51"/>
+      <c r="AQ64" s="52"/>
+      <c r="AR64" s="52"/>
+      <c r="AS64" s="53"/>
     </row>
     <row r="65" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
@@ -4454,46 +4463,46 @@
       <c r="C65" s="3"/>
       <c r="D65" s="4"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="38"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="38"/>
-      <c r="L65" s="38"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="37"/>
-      <c r="O65" s="38"/>
-      <c r="P65" s="38"/>
-      <c r="Q65" s="38"/>
-      <c r="R65" s="37"/>
-      <c r="S65" s="38"/>
-      <c r="T65" s="38"/>
-      <c r="U65" s="38"/>
-      <c r="V65" s="37"/>
-      <c r="W65" s="38"/>
-      <c r="X65" s="38"/>
-      <c r="Y65" s="38"/>
-      <c r="Z65" s="37"/>
-      <c r="AA65" s="38"/>
-      <c r="AB65" s="38"/>
-      <c r="AC65" s="38"/>
-      <c r="AD65" s="37"/>
-      <c r="AE65" s="38"/>
-      <c r="AF65" s="38"/>
-      <c r="AG65" s="38"/>
-      <c r="AH65" s="37"/>
-      <c r="AI65" s="38"/>
-      <c r="AJ65" s="38"/>
-      <c r="AK65" s="38"/>
-      <c r="AL65" s="37"/>
-      <c r="AM65" s="38"/>
-      <c r="AN65" s="38"/>
-      <c r="AO65" s="38"/>
-      <c r="AP65" s="37"/>
-      <c r="AQ65" s="38"/>
-      <c r="AR65" s="38"/>
-      <c r="AS65" s="39"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="51"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="52"/>
+      <c r="N65" s="51"/>
+      <c r="O65" s="52"/>
+      <c r="P65" s="52"/>
+      <c r="Q65" s="52"/>
+      <c r="R65" s="51"/>
+      <c r="S65" s="52"/>
+      <c r="T65" s="52"/>
+      <c r="U65" s="52"/>
+      <c r="V65" s="51"/>
+      <c r="W65" s="52"/>
+      <c r="X65" s="52"/>
+      <c r="Y65" s="52"/>
+      <c r="Z65" s="51"/>
+      <c r="AA65" s="52"/>
+      <c r="AB65" s="52"/>
+      <c r="AC65" s="52"/>
+      <c r="AD65" s="51"/>
+      <c r="AE65" s="52"/>
+      <c r="AF65" s="52"/>
+      <c r="AG65" s="52"/>
+      <c r="AH65" s="51"/>
+      <c r="AI65" s="52"/>
+      <c r="AJ65" s="52"/>
+      <c r="AK65" s="52"/>
+      <c r="AL65" s="51"/>
+      <c r="AM65" s="52"/>
+      <c r="AN65" s="52"/>
+      <c r="AO65" s="52"/>
+      <c r="AP65" s="51"/>
+      <c r="AQ65" s="52"/>
+      <c r="AR65" s="52"/>
+      <c r="AS65" s="53"/>
     </row>
     <row r="66" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
@@ -4501,70 +4510,212 @@
       <c r="C66" s="3"/>
       <c r="D66" s="4"/>
       <c r="E66" s="7"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="37"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="38"/>
-      <c r="M66" s="38"/>
-      <c r="N66" s="37"/>
-      <c r="O66" s="38"/>
-      <c r="P66" s="38"/>
-      <c r="Q66" s="38"/>
-      <c r="R66" s="37"/>
-      <c r="S66" s="38"/>
-      <c r="T66" s="38"/>
-      <c r="U66" s="38"/>
-      <c r="V66" s="37"/>
-      <c r="W66" s="38"/>
-      <c r="X66" s="38"/>
-      <c r="Y66" s="38"/>
-      <c r="Z66" s="37"/>
-      <c r="AA66" s="38"/>
-      <c r="AB66" s="38"/>
-      <c r="AC66" s="38"/>
-      <c r="AD66" s="37"/>
-      <c r="AE66" s="38"/>
-      <c r="AF66" s="38"/>
-      <c r="AG66" s="38"/>
-      <c r="AH66" s="37"/>
-      <c r="AI66" s="38"/>
-      <c r="AJ66" s="38"/>
-      <c r="AK66" s="38"/>
-      <c r="AL66" s="37"/>
-      <c r="AM66" s="38"/>
-      <c r="AN66" s="38"/>
-      <c r="AO66" s="38"/>
-      <c r="AP66" s="37"/>
-      <c r="AQ66" s="38"/>
-      <c r="AR66" s="38"/>
-      <c r="AS66" s="39"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="52"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="52"/>
+      <c r="L66" s="52"/>
+      <c r="M66" s="52"/>
+      <c r="N66" s="51"/>
+      <c r="O66" s="52"/>
+      <c r="P66" s="52"/>
+      <c r="Q66" s="52"/>
+      <c r="R66" s="51"/>
+      <c r="S66" s="52"/>
+      <c r="T66" s="52"/>
+      <c r="U66" s="52"/>
+      <c r="V66" s="51"/>
+      <c r="W66" s="52"/>
+      <c r="X66" s="52"/>
+      <c r="Y66" s="52"/>
+      <c r="Z66" s="51"/>
+      <c r="AA66" s="52"/>
+      <c r="AB66" s="52"/>
+      <c r="AC66" s="52"/>
+      <c r="AD66" s="51"/>
+      <c r="AE66" s="52"/>
+      <c r="AF66" s="52"/>
+      <c r="AG66" s="52"/>
+      <c r="AH66" s="51"/>
+      <c r="AI66" s="52"/>
+      <c r="AJ66" s="52"/>
+      <c r="AK66" s="52"/>
+      <c r="AL66" s="51"/>
+      <c r="AM66" s="52"/>
+      <c r="AN66" s="52"/>
+      <c r="AO66" s="52"/>
+      <c r="AP66" s="51"/>
+      <c r="AQ66" s="52"/>
+      <c r="AR66" s="52"/>
+      <c r="AS66" s="53"/>
     </row>
     <row r="67" spans="1:45" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="208">
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="AH62:AK62"/>
+    <mergeCell ref="AL62:AO62"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="AP66:AS66"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="AD65:AG65"/>
+    <mergeCell ref="AH65:AK65"/>
+    <mergeCell ref="AL65:AO65"/>
+    <mergeCell ref="AP65:AS65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="N66:Q66"/>
+    <mergeCell ref="R66:U66"/>
+    <mergeCell ref="V66:Y66"/>
+    <mergeCell ref="Z66:AC66"/>
+    <mergeCell ref="AD64:AG64"/>
+    <mergeCell ref="AD66:AG66"/>
+    <mergeCell ref="AH66:AK66"/>
+    <mergeCell ref="AL66:AO66"/>
+    <mergeCell ref="V65:Y65"/>
+    <mergeCell ref="Z65:AC65"/>
+    <mergeCell ref="AD63:AG63"/>
+    <mergeCell ref="AH63:AK63"/>
+    <mergeCell ref="AL63:AO63"/>
+    <mergeCell ref="AP64:AS64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="N65:Q65"/>
+    <mergeCell ref="R65:U65"/>
+    <mergeCell ref="AP63:AS63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="N64:Q64"/>
+    <mergeCell ref="R64:U64"/>
+    <mergeCell ref="V64:Y64"/>
+    <mergeCell ref="Z64:AC64"/>
+    <mergeCell ref="AH64:AK64"/>
+    <mergeCell ref="AL64:AO64"/>
+    <mergeCell ref="AP62:AS62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="N63:Q63"/>
+    <mergeCell ref="R63:U63"/>
+    <mergeCell ref="V63:Y63"/>
+    <mergeCell ref="Z63:AC63"/>
+    <mergeCell ref="AP61:AS61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="N62:Q62"/>
+    <mergeCell ref="R62:U62"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="Z62:AC62"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="N61:Q61"/>
+    <mergeCell ref="R61:U61"/>
+    <mergeCell ref="V61:Y61"/>
+    <mergeCell ref="Z61:AC61"/>
+    <mergeCell ref="AD61:AG61"/>
+    <mergeCell ref="AH61:AK61"/>
+    <mergeCell ref="AL61:AO61"/>
+    <mergeCell ref="AD62:AG62"/>
+    <mergeCell ref="AP60:AS60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="R60:U60"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="V60:Y60"/>
+    <mergeCell ref="Z60:AC60"/>
+    <mergeCell ref="AD60:AG60"/>
+    <mergeCell ref="AH60:AK60"/>
+    <mergeCell ref="AL60:AO60"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="B56:B57"/>
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="D56:D57"/>
@@ -4589,172 +4740,30 @@
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A34:A43"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="AP60:AS60"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="N60:Q60"/>
-    <mergeCell ref="R60:U60"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="V60:Y60"/>
-    <mergeCell ref="Z60:AC60"/>
-    <mergeCell ref="AD60:AG60"/>
-    <mergeCell ref="AH60:AK60"/>
-    <mergeCell ref="AL60:AO60"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="AP62:AS62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="N63:Q63"/>
-    <mergeCell ref="R63:U63"/>
-    <mergeCell ref="V63:Y63"/>
-    <mergeCell ref="Z63:AC63"/>
-    <mergeCell ref="AP61:AS61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="N62:Q62"/>
-    <mergeCell ref="R62:U62"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="Z62:AC62"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="N61:Q61"/>
-    <mergeCell ref="R61:U61"/>
-    <mergeCell ref="V61:Y61"/>
-    <mergeCell ref="Z61:AC61"/>
-    <mergeCell ref="AD61:AG61"/>
-    <mergeCell ref="AH61:AK61"/>
-    <mergeCell ref="AL61:AO61"/>
-    <mergeCell ref="AD62:AG62"/>
-    <mergeCell ref="Z65:AC65"/>
-    <mergeCell ref="AD63:AG63"/>
-    <mergeCell ref="AH63:AK63"/>
-    <mergeCell ref="AL63:AO63"/>
-    <mergeCell ref="AP64:AS64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="J65:M65"/>
-    <mergeCell ref="N65:Q65"/>
-    <mergeCell ref="R65:U65"/>
-    <mergeCell ref="AP63:AS63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="N64:Q64"/>
-    <mergeCell ref="R64:U64"/>
-    <mergeCell ref="V64:Y64"/>
-    <mergeCell ref="Z64:AC64"/>
-    <mergeCell ref="AH64:AK64"/>
-    <mergeCell ref="AL64:AO64"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B52:B53"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="AP66:AS66"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="AD65:AG65"/>
-    <mergeCell ref="AH65:AK65"/>
-    <mergeCell ref="AL65:AO65"/>
-    <mergeCell ref="AP65:AS65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="N66:Q66"/>
-    <mergeCell ref="R66:U66"/>
-    <mergeCell ref="V66:Y66"/>
-    <mergeCell ref="Z66:AC66"/>
-    <mergeCell ref="AD64:AG64"/>
-    <mergeCell ref="AD66:AG66"/>
-    <mergeCell ref="AH66:AK66"/>
-    <mergeCell ref="AL66:AO66"/>
-    <mergeCell ref="V65:Y65"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="AH62:AK62"/>
-    <mergeCell ref="AL62:AO62"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
day-7 without day-6 journal will be added
</commit_message>
<xml_diff>
--- a/Ege Zeitplan.xlsx
+++ b/Ege Zeitplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\010-IPA\IPA-Dokumentation\Tag6\IPA-Dok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\010-IPA\IPA-Dokumentation\Tag7\IPA-Dok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884A24F4-03E1-43C7-8CE3-0DFC04E5F7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E680B846-99BC-4442-B6C2-2A4F8664C071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB9C6447-36BB-4D67-BBCE-08BA330606A4}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -680,107 +680,101 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46E2A04-0C7F-49B8-B0E7-B380E8D10631}">
   <dimension ref="A1:AS67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC41" sqref="AC41"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,151 +1125,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="43" t="s">
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="43" t="s">
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="43" t="s">
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="43" t="s">
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="43" t="s">
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="43" t="s">
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="43" t="s">
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="43" t="s">
+      <c r="AI1" s="42"/>
+      <c r="AJ1" s="42"/>
+      <c r="AK1" s="42"/>
+      <c r="AL1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="43" t="s">
+      <c r="AM1" s="42"/>
+      <c r="AN1" s="42"/>
+      <c r="AO1" s="42"/>
+      <c r="AP1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="45"/>
+      <c r="AQ1" s="42"/>
+      <c r="AR1" s="42"/>
+      <c r="AS1" s="43"/>
     </row>
     <row r="2" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="37" t="s">
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="37" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="37" t="s">
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="37" t="s">
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="37" t="s">
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="37" t="s">
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="38"/>
-      <c r="AD2" s="37" t="s">
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" s="38"/>
-      <c r="AF2" s="38"/>
-      <c r="AG2" s="38"/>
-      <c r="AH2" s="37" t="s">
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="AI2" s="38"/>
-      <c r="AJ2" s="38"/>
-      <c r="AK2" s="38"/>
-      <c r="AL2" s="37" t="s">
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
+      <c r="AL2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AM2" s="38"/>
-      <c r="AN2" s="38"/>
-      <c r="AO2" s="38"/>
-      <c r="AP2" s="37" t="s">
+      <c r="AM2" s="36"/>
+      <c r="AN2" s="36"/>
+      <c r="AO2" s="36"/>
+      <c r="AP2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="AQ2" s="38"/>
-      <c r="AR2" s="38"/>
-      <c r="AS2" s="39"/>
+      <c r="AQ2" s="36"/>
+      <c r="AR2" s="36"/>
+      <c r="AS2" s="37"/>
     </row>
     <row r="3" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1405,16 +1399,16 @@
     </row>
     <row r="4" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="32">
         <v>9</v>
       </c>
-      <c r="E4" s="46"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -1458,10 +1452,10 @@
     </row>
     <row r="5" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="45"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -1505,16 +1499,16 @@
     </row>
     <row r="6" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28"/>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="32">
         <v>2</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="32">
         <v>2</v>
       </c>
       <c r="F6" s="5"/>
@@ -1560,10 +1554,10 @@
     </row>
     <row r="7" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1607,16 +1601,16 @@
     </row>
     <row r="8" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28"/>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="32">
         <v>2</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1660,10 +1654,10 @@
     </row>
     <row r="9" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1707,16 +1701,16 @@
     </row>
     <row r="10" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="28"/>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="32">
         <v>1</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="32">
         <v>1</v>
       </c>
       <c r="F10" s="10"/>
@@ -1762,10 +1756,10 @@
     </row>
     <row r="11" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="18"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
@@ -1811,16 +1805,16 @@
       <c r="A12" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="32">
         <v>1</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="32">
         <v>1</v>
       </c>
       <c r="F12" s="5"/>
@@ -1866,10 +1860,10 @@
     </row>
     <row r="13" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1913,16 +1907,16 @@
     </row>
     <row r="14" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28"/>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="32">
         <v>1</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="32">
         <v>1</v>
       </c>
       <c r="F14" s="5"/>
@@ -1968,10 +1962,10 @@
     </row>
     <row r="15" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="5"/>
       <c r="G15" s="12"/>
       <c r="H15" s="5"/>
@@ -2015,16 +2009,16 @@
     </row>
     <row r="16" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28"/>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="32">
         <v>2</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="32">
         <v>2</v>
       </c>
       <c r="F16" s="5"/>
@@ -2070,10 +2064,10 @@
     </row>
     <row r="17" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="15"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
@@ -2119,16 +2113,16 @@
       <c r="A18" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="32">
         <v>4</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="32">
         <v>4.5</v>
       </c>
       <c r="F18" s="5"/>
@@ -2174,10 +2168,10 @@
     </row>
     <row r="19" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="12"/>
@@ -2221,16 +2215,16 @@
     </row>
     <row r="20" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28"/>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="32">
         <v>2</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="32">
         <v>2</v>
       </c>
       <c r="F20" s="5"/>
@@ -2276,10 +2270,10 @@
     </row>
     <row r="21" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="28"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -2323,16 +2317,16 @@
     </row>
     <row r="22" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="28"/>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="32">
         <v>2</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="32">
         <v>2</v>
       </c>
       <c r="F22" s="5"/>
@@ -2378,10 +2372,10 @@
     </row>
     <row r="23" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="28"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -2425,16 +2419,16 @@
     </row>
     <row r="24" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="28"/>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="32">
         <v>2</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="32">
         <v>2</v>
       </c>
       <c r="F24" s="5"/>
@@ -2480,10 +2474,10 @@
     </row>
     <row r="25" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="28"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -2527,16 +2521,16 @@
     </row>
     <row r="26" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="28"/>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="32">
         <v>2</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="32">
         <v>1</v>
       </c>
       <c r="F26" s="5"/>
@@ -2582,10 +2576,10 @@
     </row>
     <row r="27" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="28"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -2629,16 +2623,16 @@
     </row>
     <row r="28" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="28"/>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="32">
         <v>2</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="32">
         <v>2</v>
       </c>
       <c r="F28" s="5"/>
@@ -2684,10 +2678,10 @@
     </row>
     <row r="29" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="29"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -2733,16 +2727,16 @@
       <c r="A30" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="32">
         <v>1</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="32">
         <v>1</v>
       </c>
       <c r="F30" s="5"/>
@@ -2788,10 +2782,10 @@
     </row>
     <row r="31" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="28"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -2835,16 +2829,16 @@
     </row>
     <row r="32" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="28"/>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="32">
         <v>1</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="32">
         <v>1</v>
       </c>
       <c r="F32" s="5"/>
@@ -2890,10 +2884,10 @@
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="29"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -2939,16 +2933,16 @@
       <c r="A34" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="32">
         <v>2</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="32">
         <v>1</v>
       </c>
       <c r="F34" s="5"/>
@@ -2994,10 +2988,10 @@
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="28"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -3041,16 +3035,16 @@
     </row>
     <row r="36" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="28"/>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="32">
         <v>8.75</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="32">
         <v>10.75</v>
       </c>
       <c r="F36" s="5"/>
@@ -3096,10 +3090,10 @@
     </row>
     <row r="37" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="28"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
@@ -3143,16 +3137,18 @@
     </row>
     <row r="38" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="28"/>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="32">
         <v>8</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="32">
+        <v>6</v>
+      </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
@@ -3196,10 +3192,10 @@
     </row>
     <row r="39" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="28"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
@@ -3243,16 +3239,18 @@
     </row>
     <row r="40" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="28"/>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="32">
         <v>2</v>
       </c>
-      <c r="E40" s="23"/>
+      <c r="E40" s="32">
+        <v>2</v>
+      </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
@@ -3274,10 +3272,10 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="9"/>
       <c r="Z40" s="5"/>
-      <c r="AA40" s="55"/>
-      <c r="AB40" s="55"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="5"/>
       <c r="AC40" s="11"/>
-      <c r="AD40" s="55"/>
+      <c r="AD40" s="5"/>
       <c r="AE40" s="5"/>
       <c r="AF40" s="5"/>
       <c r="AG40" s="9"/>
@@ -3296,10 +3294,10 @@
     </row>
     <row r="41" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="28"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -3322,7 +3320,7 @@
       <c r="Y41" s="9"/>
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
-      <c r="AB41" s="55"/>
+      <c r="AB41" s="5"/>
       <c r="AC41" s="13"/>
       <c r="AD41" s="5"/>
       <c r="AE41" s="5"/>
@@ -3343,16 +3341,18 @@
     </row>
     <row r="42" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="28"/>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="23">
+      <c r="D42" s="32">
         <v>2</v>
       </c>
-      <c r="E42" s="23"/>
+      <c r="E42" s="32">
+        <v>2</v>
+      </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
@@ -3376,7 +3376,7 @@
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
       <c r="AB42" s="5"/>
-      <c r="AC42" s="56"/>
+      <c r="AC42" s="9"/>
       <c r="AD42" s="10"/>
       <c r="AE42" s="5"/>
       <c r="AF42" s="5"/>
@@ -3396,10 +3396,10 @@
     </row>
     <row r="43" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="28"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
@@ -3424,7 +3424,7 @@
       <c r="AA43" s="5"/>
       <c r="AB43" s="5"/>
       <c r="AC43" s="9"/>
-      <c r="AD43" s="5"/>
+      <c r="AD43" s="12"/>
       <c r="AE43" s="5"/>
       <c r="AF43" s="5"/>
       <c r="AG43" s="9"/>
@@ -3445,16 +3445,18 @@
       <c r="A44" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="23">
+      <c r="D44" s="32">
         <v>2</v>
       </c>
-      <c r="E44" s="23"/>
+      <c r="E44" s="32">
+        <v>2</v>
+      </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
@@ -3498,10 +3500,10 @@
     </row>
     <row r="45" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="28"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -3527,7 +3529,7 @@
       <c r="AB45" s="5"/>
       <c r="AC45" s="9"/>
       <c r="AD45" s="5"/>
-      <c r="AE45" s="5"/>
+      <c r="AE45" s="12"/>
       <c r="AF45" s="5"/>
       <c r="AG45" s="9"/>
       <c r="AH45" s="5"/>
@@ -3545,16 +3547,18 @@
     </row>
     <row r="46" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="28"/>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D46" s="23">
+      <c r="D46" s="32">
         <v>8</v>
       </c>
-      <c r="E46" s="23"/>
+      <c r="E46" s="32">
+        <v>4</v>
+      </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
@@ -3598,10 +3602,10 @@
     </row>
     <row r="47" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="29"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
@@ -3628,8 +3632,8 @@
       <c r="AC47" s="9"/>
       <c r="AD47" s="5"/>
       <c r="AE47" s="5"/>
-      <c r="AF47" s="5"/>
-      <c r="AG47" s="9"/>
+      <c r="AF47" s="12"/>
+      <c r="AG47" s="13"/>
       <c r="AH47" s="5"/>
       <c r="AI47" s="5"/>
       <c r="AJ47" s="5"/>
@@ -3644,19 +3648,19 @@
       <c r="AS47" s="9"/>
     </row>
     <row r="48" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="52" t="s">
+      <c r="A48" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D48" s="23">
+      <c r="D48" s="32">
         <v>2</v>
       </c>
-      <c r="E48" s="23"/>
+      <c r="E48" s="32"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
@@ -3699,11 +3703,11 @@
       <c r="AS48" s="9"/>
     </row>
     <row r="49" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="53"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
@@ -3746,17 +3750,17 @@
       <c r="AS49" s="9"/>
     </row>
     <row r="50" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="53"/>
-      <c r="B50" s="30" t="s">
+      <c r="A50" s="34"/>
+      <c r="B50" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="23">
+      <c r="D50" s="32">
         <v>2</v>
       </c>
-      <c r="E50" s="23"/>
+      <c r="E50" s="32"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
@@ -3799,11 +3803,11 @@
       <c r="AS50" s="9"/>
     </row>
     <row r="51" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="53"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
@@ -3846,17 +3850,17 @@
       <c r="AS51" s="9"/>
     </row>
     <row r="52" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="53"/>
-      <c r="B52" s="30" t="s">
+      <c r="A52" s="34"/>
+      <c r="B52" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D52" s="23">
+      <c r="D52" s="32">
         <v>2</v>
       </c>
-      <c r="E52" s="23"/>
+      <c r="E52" s="32"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
@@ -3899,11 +3903,11 @@
       <c r="AS52" s="9"/>
     </row>
     <row r="53" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="53"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
@@ -3946,17 +3950,17 @@
       <c r="AS53" s="9"/>
     </row>
     <row r="54" spans="1:45" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="53"/>
-      <c r="B54" s="30" t="s">
+      <c r="A54" s="34"/>
+      <c r="B54" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C54" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="D54" s="23">
+      <c r="D54" s="32">
         <v>2</v>
       </c>
-      <c r="E54" s="23"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
@@ -3999,11 +4003,11 @@
       <c r="AS54" s="9"/>
     </row>
     <row r="55" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="53"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
@@ -4046,17 +4050,17 @@
       <c r="AS55" s="9"/>
     </row>
     <row r="56" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="53"/>
-      <c r="B56" s="30" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="25" t="s">
+      <c r="C56" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D56" s="23">
+      <c r="D56" s="32">
         <v>2</v>
       </c>
-      <c r="E56" s="23"/>
+      <c r="E56" s="32"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
@@ -4099,11 +4103,11 @@
       <c r="AS56" s="9"/>
     </row>
     <row r="57" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="54"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
@@ -4146,17 +4150,17 @@
       <c r="AS57" s="9"/>
     </row>
     <row r="58" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="52"/>
-      <c r="B58" s="30" t="s">
+      <c r="A58" s="25"/>
+      <c r="B58" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="25" t="s">
+      <c r="C58" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D58" s="23">
+      <c r="D58" s="32">
         <v>4</v>
       </c>
-      <c r="E58" s="23"/>
+      <c r="E58" s="32"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
@@ -4193,17 +4197,17 @@
       <c r="AM58" s="5"/>
       <c r="AN58" s="5"/>
       <c r="AO58" s="9"/>
-      <c r="AP58" s="55"/>
+      <c r="AP58" s="5"/>
       <c r="AQ58" s="10"/>
       <c r="AR58" s="10"/>
       <c r="AS58" s="9"/>
     </row>
     <row r="59" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="54"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
@@ -4256,46 +4260,46 @@
         <v>80.75</v>
       </c>
       <c r="E60" s="6"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="35"/>
-      <c r="N60" s="34"/>
-      <c r="O60" s="35"/>
-      <c r="P60" s="35"/>
-      <c r="Q60" s="35"/>
-      <c r="R60" s="34"/>
-      <c r="S60" s="35"/>
-      <c r="T60" s="35"/>
-      <c r="U60" s="35"/>
-      <c r="V60" s="34"/>
-      <c r="W60" s="35"/>
-      <c r="X60" s="35"/>
-      <c r="Y60" s="35"/>
-      <c r="Z60" s="34"/>
-      <c r="AA60" s="35"/>
-      <c r="AB60" s="35"/>
-      <c r="AC60" s="35"/>
-      <c r="AD60" s="34"/>
-      <c r="AE60" s="35"/>
-      <c r="AF60" s="35"/>
-      <c r="AG60" s="35"/>
-      <c r="AH60" s="34"/>
-      <c r="AI60" s="35"/>
-      <c r="AJ60" s="35"/>
-      <c r="AK60" s="35"/>
-      <c r="AL60" s="34"/>
-      <c r="AM60" s="35"/>
-      <c r="AN60" s="35"/>
-      <c r="AO60" s="35"/>
-      <c r="AP60" s="34"/>
-      <c r="AQ60" s="35"/>
-      <c r="AR60" s="35"/>
-      <c r="AS60" s="36"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="51"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="50"/>
+      <c r="K60" s="51"/>
+      <c r="L60" s="51"/>
+      <c r="M60" s="51"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="51"/>
+      <c r="P60" s="51"/>
+      <c r="Q60" s="51"/>
+      <c r="R60" s="50"/>
+      <c r="S60" s="51"/>
+      <c r="T60" s="51"/>
+      <c r="U60" s="51"/>
+      <c r="V60" s="50"/>
+      <c r="W60" s="51"/>
+      <c r="X60" s="51"/>
+      <c r="Y60" s="51"/>
+      <c r="Z60" s="50"/>
+      <c r="AA60" s="51"/>
+      <c r="AB60" s="51"/>
+      <c r="AC60" s="51"/>
+      <c r="AD60" s="50"/>
+      <c r="AE60" s="51"/>
+      <c r="AF60" s="51"/>
+      <c r="AG60" s="51"/>
+      <c r="AH60" s="50"/>
+      <c r="AI60" s="51"/>
+      <c r="AJ60" s="51"/>
+      <c r="AK60" s="51"/>
+      <c r="AL60" s="50"/>
+      <c r="AM60" s="51"/>
+      <c r="AN60" s="51"/>
+      <c r="AO60" s="51"/>
+      <c r="AP60" s="50"/>
+      <c r="AQ60" s="51"/>
+      <c r="AR60" s="51"/>
+      <c r="AS60" s="52"/>
     </row>
     <row r="61" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
@@ -4303,46 +4307,46 @@
       <c r="C61" s="6"/>
       <c r="D61" s="3"/>
       <c r="E61" s="6"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="35"/>
-      <c r="N61" s="34"/>
-      <c r="O61" s="35"/>
-      <c r="P61" s="35"/>
-      <c r="Q61" s="35"/>
-      <c r="R61" s="34"/>
-      <c r="S61" s="35"/>
-      <c r="T61" s="35"/>
-      <c r="U61" s="35"/>
-      <c r="V61" s="34"/>
-      <c r="W61" s="35"/>
-      <c r="X61" s="35"/>
-      <c r="Y61" s="35"/>
-      <c r="Z61" s="34"/>
-      <c r="AA61" s="35"/>
-      <c r="AB61" s="35"/>
-      <c r="AC61" s="35"/>
-      <c r="AD61" s="34"/>
-      <c r="AE61" s="35"/>
-      <c r="AF61" s="35"/>
-      <c r="AG61" s="35"/>
-      <c r="AH61" s="34"/>
-      <c r="AI61" s="35"/>
-      <c r="AJ61" s="35"/>
-      <c r="AK61" s="35"/>
-      <c r="AL61" s="34"/>
-      <c r="AM61" s="35"/>
-      <c r="AN61" s="35"/>
-      <c r="AO61" s="35"/>
-      <c r="AP61" s="34"/>
-      <c r="AQ61" s="35"/>
-      <c r="AR61" s="35"/>
-      <c r="AS61" s="36"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="51"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="51"/>
+      <c r="L61" s="51"/>
+      <c r="M61" s="51"/>
+      <c r="N61" s="50"/>
+      <c r="O61" s="51"/>
+      <c r="P61" s="51"/>
+      <c r="Q61" s="51"/>
+      <c r="R61" s="50"/>
+      <c r="S61" s="51"/>
+      <c r="T61" s="51"/>
+      <c r="U61" s="51"/>
+      <c r="V61" s="50"/>
+      <c r="W61" s="51"/>
+      <c r="X61" s="51"/>
+      <c r="Y61" s="51"/>
+      <c r="Z61" s="50"/>
+      <c r="AA61" s="51"/>
+      <c r="AB61" s="51"/>
+      <c r="AC61" s="51"/>
+      <c r="AD61" s="50"/>
+      <c r="AE61" s="51"/>
+      <c r="AF61" s="51"/>
+      <c r="AG61" s="51"/>
+      <c r="AH61" s="50"/>
+      <c r="AI61" s="51"/>
+      <c r="AJ61" s="51"/>
+      <c r="AK61" s="51"/>
+      <c r="AL61" s="50"/>
+      <c r="AM61" s="51"/>
+      <c r="AN61" s="51"/>
+      <c r="AO61" s="51"/>
+      <c r="AP61" s="50"/>
+      <c r="AQ61" s="51"/>
+      <c r="AR61" s="51"/>
+      <c r="AS61" s="52"/>
     </row>
     <row r="62" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
@@ -4352,46 +4356,46 @@
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="6"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="34"/>
-      <c r="K62" s="35"/>
-      <c r="L62" s="35"/>
-      <c r="M62" s="35"/>
-      <c r="N62" s="34"/>
-      <c r="O62" s="35"/>
-      <c r="P62" s="35"/>
-      <c r="Q62" s="35"/>
-      <c r="R62" s="34"/>
-      <c r="S62" s="35"/>
-      <c r="T62" s="35"/>
-      <c r="U62" s="35"/>
-      <c r="V62" s="34"/>
-      <c r="W62" s="35"/>
-      <c r="X62" s="35"/>
-      <c r="Y62" s="35"/>
-      <c r="Z62" s="34"/>
-      <c r="AA62" s="35"/>
-      <c r="AB62" s="35"/>
-      <c r="AC62" s="35"/>
-      <c r="AD62" s="34"/>
-      <c r="AE62" s="35"/>
-      <c r="AF62" s="35"/>
-      <c r="AG62" s="35"/>
-      <c r="AH62" s="34"/>
-      <c r="AI62" s="35"/>
-      <c r="AJ62" s="35"/>
-      <c r="AK62" s="35"/>
-      <c r="AL62" s="34"/>
-      <c r="AM62" s="35"/>
-      <c r="AN62" s="35"/>
-      <c r="AO62" s="35"/>
-      <c r="AP62" s="34"/>
-      <c r="AQ62" s="35"/>
-      <c r="AR62" s="35"/>
-      <c r="AS62" s="36"/>
+      <c r="F62" s="50"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="50"/>
+      <c r="K62" s="51"/>
+      <c r="L62" s="51"/>
+      <c r="M62" s="51"/>
+      <c r="N62" s="50"/>
+      <c r="O62" s="51"/>
+      <c r="P62" s="51"/>
+      <c r="Q62" s="51"/>
+      <c r="R62" s="50"/>
+      <c r="S62" s="51"/>
+      <c r="T62" s="51"/>
+      <c r="U62" s="51"/>
+      <c r="V62" s="50"/>
+      <c r="W62" s="51"/>
+      <c r="X62" s="51"/>
+      <c r="Y62" s="51"/>
+      <c r="Z62" s="50"/>
+      <c r="AA62" s="51"/>
+      <c r="AB62" s="51"/>
+      <c r="AC62" s="51"/>
+      <c r="AD62" s="50"/>
+      <c r="AE62" s="51"/>
+      <c r="AF62" s="51"/>
+      <c r="AG62" s="51"/>
+      <c r="AH62" s="50"/>
+      <c r="AI62" s="51"/>
+      <c r="AJ62" s="51"/>
+      <c r="AK62" s="51"/>
+      <c r="AL62" s="50"/>
+      <c r="AM62" s="51"/>
+      <c r="AN62" s="51"/>
+      <c r="AO62" s="51"/>
+      <c r="AP62" s="50"/>
+      <c r="AQ62" s="51"/>
+      <c r="AR62" s="51"/>
+      <c r="AS62" s="52"/>
     </row>
     <row r="63" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
@@ -4399,46 +4403,46 @@
       <c r="C63" s="2"/>
       <c r="D63" s="3"/>
       <c r="E63" s="6"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="34"/>
-      <c r="O63" s="35"/>
-      <c r="P63" s="35"/>
-      <c r="Q63" s="35"/>
-      <c r="R63" s="34"/>
-      <c r="S63" s="35"/>
-      <c r="T63" s="35"/>
-      <c r="U63" s="35"/>
-      <c r="V63" s="34"/>
-      <c r="W63" s="35"/>
-      <c r="X63" s="35"/>
-      <c r="Y63" s="35"/>
-      <c r="Z63" s="34"/>
-      <c r="AA63" s="35"/>
-      <c r="AB63" s="35"/>
-      <c r="AC63" s="35"/>
-      <c r="AD63" s="34"/>
-      <c r="AE63" s="35"/>
-      <c r="AF63" s="35"/>
-      <c r="AG63" s="35"/>
-      <c r="AH63" s="34"/>
-      <c r="AI63" s="35"/>
-      <c r="AJ63" s="35"/>
-      <c r="AK63" s="35"/>
-      <c r="AL63" s="34"/>
-      <c r="AM63" s="35"/>
-      <c r="AN63" s="35"/>
-      <c r="AO63" s="35"/>
-      <c r="AP63" s="34"/>
-      <c r="AQ63" s="35"/>
-      <c r="AR63" s="35"/>
-      <c r="AS63" s="36"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="51"/>
+      <c r="J63" s="50"/>
+      <c r="K63" s="51"/>
+      <c r="L63" s="51"/>
+      <c r="M63" s="51"/>
+      <c r="N63" s="50"/>
+      <c r="O63" s="51"/>
+      <c r="P63" s="51"/>
+      <c r="Q63" s="51"/>
+      <c r="R63" s="50"/>
+      <c r="S63" s="51"/>
+      <c r="T63" s="51"/>
+      <c r="U63" s="51"/>
+      <c r="V63" s="50"/>
+      <c r="W63" s="51"/>
+      <c r="X63" s="51"/>
+      <c r="Y63" s="51"/>
+      <c r="Z63" s="50"/>
+      <c r="AA63" s="51"/>
+      <c r="AB63" s="51"/>
+      <c r="AC63" s="51"/>
+      <c r="AD63" s="50"/>
+      <c r="AE63" s="51"/>
+      <c r="AF63" s="51"/>
+      <c r="AG63" s="51"/>
+      <c r="AH63" s="50"/>
+      <c r="AI63" s="51"/>
+      <c r="AJ63" s="51"/>
+      <c r="AK63" s="51"/>
+      <c r="AL63" s="50"/>
+      <c r="AM63" s="51"/>
+      <c r="AN63" s="51"/>
+      <c r="AO63" s="51"/>
+      <c r="AP63" s="50"/>
+      <c r="AQ63" s="51"/>
+      <c r="AR63" s="51"/>
+      <c r="AS63" s="52"/>
     </row>
     <row r="64" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
@@ -4446,46 +4450,46 @@
       <c r="C64" s="2"/>
       <c r="D64" s="3"/>
       <c r="E64" s="6"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="34"/>
-      <c r="K64" s="35"/>
-      <c r="L64" s="35"/>
-      <c r="M64" s="35"/>
-      <c r="N64" s="34"/>
-      <c r="O64" s="35"/>
-      <c r="P64" s="35"/>
-      <c r="Q64" s="35"/>
-      <c r="R64" s="34"/>
-      <c r="S64" s="35"/>
-      <c r="T64" s="35"/>
-      <c r="U64" s="35"/>
-      <c r="V64" s="34"/>
-      <c r="W64" s="35"/>
-      <c r="X64" s="35"/>
-      <c r="Y64" s="35"/>
-      <c r="Z64" s="34"/>
-      <c r="AA64" s="35"/>
-      <c r="AB64" s="35"/>
-      <c r="AC64" s="35"/>
-      <c r="AD64" s="34"/>
-      <c r="AE64" s="35"/>
-      <c r="AF64" s="35"/>
-      <c r="AG64" s="35"/>
-      <c r="AH64" s="34"/>
-      <c r="AI64" s="35"/>
-      <c r="AJ64" s="35"/>
-      <c r="AK64" s="35"/>
-      <c r="AL64" s="34"/>
-      <c r="AM64" s="35"/>
-      <c r="AN64" s="35"/>
-      <c r="AO64" s="35"/>
-      <c r="AP64" s="34"/>
-      <c r="AQ64" s="35"/>
-      <c r="AR64" s="35"/>
-      <c r="AS64" s="36"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="51"/>
+      <c r="I64" s="51"/>
+      <c r="J64" s="50"/>
+      <c r="K64" s="51"/>
+      <c r="L64" s="51"/>
+      <c r="M64" s="51"/>
+      <c r="N64" s="50"/>
+      <c r="O64" s="51"/>
+      <c r="P64" s="51"/>
+      <c r="Q64" s="51"/>
+      <c r="R64" s="50"/>
+      <c r="S64" s="51"/>
+      <c r="T64" s="51"/>
+      <c r="U64" s="51"/>
+      <c r="V64" s="50"/>
+      <c r="W64" s="51"/>
+      <c r="X64" s="51"/>
+      <c r="Y64" s="51"/>
+      <c r="Z64" s="50"/>
+      <c r="AA64" s="51"/>
+      <c r="AB64" s="51"/>
+      <c r="AC64" s="51"/>
+      <c r="AD64" s="50"/>
+      <c r="AE64" s="51"/>
+      <c r="AF64" s="51"/>
+      <c r="AG64" s="51"/>
+      <c r="AH64" s="50"/>
+      <c r="AI64" s="51"/>
+      <c r="AJ64" s="51"/>
+      <c r="AK64" s="51"/>
+      <c r="AL64" s="50"/>
+      <c r="AM64" s="51"/>
+      <c r="AN64" s="51"/>
+      <c r="AO64" s="51"/>
+      <c r="AP64" s="50"/>
+      <c r="AQ64" s="51"/>
+      <c r="AR64" s="51"/>
+      <c r="AS64" s="52"/>
     </row>
     <row r="65" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
@@ -4493,46 +4497,46 @@
       <c r="C65" s="2"/>
       <c r="D65" s="3"/>
       <c r="E65" s="6"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="34"/>
-      <c r="K65" s="35"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="34"/>
-      <c r="O65" s="35"/>
-      <c r="P65" s="35"/>
-      <c r="Q65" s="35"/>
-      <c r="R65" s="34"/>
-      <c r="S65" s="35"/>
-      <c r="T65" s="35"/>
-      <c r="U65" s="35"/>
-      <c r="V65" s="34"/>
-      <c r="W65" s="35"/>
-      <c r="X65" s="35"/>
-      <c r="Y65" s="35"/>
-      <c r="Z65" s="34"/>
-      <c r="AA65" s="35"/>
-      <c r="AB65" s="35"/>
-      <c r="AC65" s="35"/>
-      <c r="AD65" s="34"/>
-      <c r="AE65" s="35"/>
-      <c r="AF65" s="35"/>
-      <c r="AG65" s="35"/>
-      <c r="AH65" s="34"/>
-      <c r="AI65" s="35"/>
-      <c r="AJ65" s="35"/>
-      <c r="AK65" s="35"/>
-      <c r="AL65" s="34"/>
-      <c r="AM65" s="35"/>
-      <c r="AN65" s="35"/>
-      <c r="AO65" s="35"/>
-      <c r="AP65" s="34"/>
-      <c r="AQ65" s="35"/>
-      <c r="AR65" s="35"/>
-      <c r="AS65" s="36"/>
+      <c r="F65" s="50"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="51"/>
+      <c r="J65" s="50"/>
+      <c r="K65" s="51"/>
+      <c r="L65" s="51"/>
+      <c r="M65" s="51"/>
+      <c r="N65" s="50"/>
+      <c r="O65" s="51"/>
+      <c r="P65" s="51"/>
+      <c r="Q65" s="51"/>
+      <c r="R65" s="50"/>
+      <c r="S65" s="51"/>
+      <c r="T65" s="51"/>
+      <c r="U65" s="51"/>
+      <c r="V65" s="50"/>
+      <c r="W65" s="51"/>
+      <c r="X65" s="51"/>
+      <c r="Y65" s="51"/>
+      <c r="Z65" s="50"/>
+      <c r="AA65" s="51"/>
+      <c r="AB65" s="51"/>
+      <c r="AC65" s="51"/>
+      <c r="AD65" s="50"/>
+      <c r="AE65" s="51"/>
+      <c r="AF65" s="51"/>
+      <c r="AG65" s="51"/>
+      <c r="AH65" s="50"/>
+      <c r="AI65" s="51"/>
+      <c r="AJ65" s="51"/>
+      <c r="AK65" s="51"/>
+      <c r="AL65" s="50"/>
+      <c r="AM65" s="51"/>
+      <c r="AN65" s="51"/>
+      <c r="AO65" s="51"/>
+      <c r="AP65" s="50"/>
+      <c r="AQ65" s="51"/>
+      <c r="AR65" s="51"/>
+      <c r="AS65" s="52"/>
     </row>
     <row r="66" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
@@ -4540,102 +4544,184 @@
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
       <c r="E66" s="6"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="35"/>
-      <c r="J66" s="34"/>
-      <c r="K66" s="35"/>
-      <c r="L66" s="35"/>
-      <c r="M66" s="35"/>
-      <c r="N66" s="34"/>
-      <c r="O66" s="35"/>
-      <c r="P66" s="35"/>
-      <c r="Q66" s="35"/>
-      <c r="R66" s="34"/>
-      <c r="S66" s="35"/>
-      <c r="T66" s="35"/>
-      <c r="U66" s="35"/>
-      <c r="V66" s="34"/>
-      <c r="W66" s="35"/>
-      <c r="X66" s="35"/>
-      <c r="Y66" s="35"/>
-      <c r="Z66" s="34"/>
-      <c r="AA66" s="35"/>
-      <c r="AB66" s="35"/>
-      <c r="AC66" s="35"/>
-      <c r="AD66" s="34"/>
-      <c r="AE66" s="35"/>
-      <c r="AF66" s="35"/>
-      <c r="AG66" s="35"/>
-      <c r="AH66" s="34"/>
-      <c r="AI66" s="35"/>
-      <c r="AJ66" s="35"/>
-      <c r="AK66" s="35"/>
-      <c r="AL66" s="34"/>
-      <c r="AM66" s="35"/>
-      <c r="AN66" s="35"/>
-      <c r="AO66" s="35"/>
-      <c r="AP66" s="34"/>
-      <c r="AQ66" s="35"/>
-      <c r="AR66" s="35"/>
-      <c r="AS66" s="36"/>
+      <c r="F66" s="50"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="50"/>
+      <c r="K66" s="51"/>
+      <c r="L66" s="51"/>
+      <c r="M66" s="51"/>
+      <c r="N66" s="50"/>
+      <c r="O66" s="51"/>
+      <c r="P66" s="51"/>
+      <c r="Q66" s="51"/>
+      <c r="R66" s="50"/>
+      <c r="S66" s="51"/>
+      <c r="T66" s="51"/>
+      <c r="U66" s="51"/>
+      <c r="V66" s="50"/>
+      <c r="W66" s="51"/>
+      <c r="X66" s="51"/>
+      <c r="Y66" s="51"/>
+      <c r="Z66" s="50"/>
+      <c r="AA66" s="51"/>
+      <c r="AB66" s="51"/>
+      <c r="AC66" s="51"/>
+      <c r="AD66" s="50"/>
+      <c r="AE66" s="51"/>
+      <c r="AF66" s="51"/>
+      <c r="AG66" s="51"/>
+      <c r="AH66" s="50"/>
+      <c r="AI66" s="51"/>
+      <c r="AJ66" s="51"/>
+      <c r="AK66" s="51"/>
+      <c r="AL66" s="50"/>
+      <c r="AM66" s="51"/>
+      <c r="AN66" s="51"/>
+      <c r="AO66" s="51"/>
+      <c r="AP66" s="50"/>
+      <c r="AQ66" s="51"/>
+      <c r="AR66" s="51"/>
+      <c r="AS66" s="52"/>
     </row>
     <row r="67" spans="1:45" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="214">
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="A48:A57"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="AH62:AK62"/>
+    <mergeCell ref="AL62:AO62"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="AP66:AS66"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="AD65:AG65"/>
+    <mergeCell ref="AH65:AK65"/>
+    <mergeCell ref="AL65:AO65"/>
+    <mergeCell ref="AP65:AS65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="N66:Q66"/>
+    <mergeCell ref="R66:U66"/>
+    <mergeCell ref="V66:Y66"/>
+    <mergeCell ref="Z66:AC66"/>
+    <mergeCell ref="AD64:AG64"/>
+    <mergeCell ref="AD66:AG66"/>
+    <mergeCell ref="AH66:AK66"/>
+    <mergeCell ref="AL66:AO66"/>
+    <mergeCell ref="V65:Y65"/>
+    <mergeCell ref="Z65:AC65"/>
+    <mergeCell ref="AD63:AG63"/>
+    <mergeCell ref="AH63:AK63"/>
+    <mergeCell ref="AL63:AO63"/>
+    <mergeCell ref="AP64:AS64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="N65:Q65"/>
+    <mergeCell ref="R65:U65"/>
+    <mergeCell ref="AP63:AS63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="N64:Q64"/>
+    <mergeCell ref="R64:U64"/>
+    <mergeCell ref="V64:Y64"/>
+    <mergeCell ref="Z64:AC64"/>
+    <mergeCell ref="AH64:AK64"/>
+    <mergeCell ref="AL64:AO64"/>
+    <mergeCell ref="AP62:AS62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="N63:Q63"/>
+    <mergeCell ref="R63:U63"/>
+    <mergeCell ref="V63:Y63"/>
+    <mergeCell ref="Z63:AC63"/>
+    <mergeCell ref="AP61:AS61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="N62:Q62"/>
+    <mergeCell ref="R62:U62"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="Z62:AC62"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="N61:Q61"/>
+    <mergeCell ref="R61:U61"/>
+    <mergeCell ref="V61:Y61"/>
+    <mergeCell ref="Z61:AC61"/>
+    <mergeCell ref="AD61:AG61"/>
+    <mergeCell ref="AH61:AK61"/>
+    <mergeCell ref="AL61:AO61"/>
+    <mergeCell ref="AD62:AG62"/>
+    <mergeCell ref="AP60:AS60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="R60:U60"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="V60:Y60"/>
+    <mergeCell ref="Z60:AC60"/>
+    <mergeCell ref="AD60:AG60"/>
+    <mergeCell ref="AH60:AK60"/>
+    <mergeCell ref="AL60:AO60"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="E52:E53"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
@@ -4660,146 +4746,64 @@
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:E2"/>
     <mergeCell ref="A4:A11"/>
-    <mergeCell ref="AP60:AS60"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="N60:Q60"/>
-    <mergeCell ref="R60:U60"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="V60:Y60"/>
-    <mergeCell ref="Z60:AC60"/>
-    <mergeCell ref="AD60:AG60"/>
-    <mergeCell ref="AH60:AK60"/>
-    <mergeCell ref="AL60:AO60"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="AP62:AS62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="N63:Q63"/>
-    <mergeCell ref="R63:U63"/>
-    <mergeCell ref="V63:Y63"/>
-    <mergeCell ref="Z63:AC63"/>
-    <mergeCell ref="AP61:AS61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="N62:Q62"/>
-    <mergeCell ref="R62:U62"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="Z62:AC62"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="N61:Q61"/>
-    <mergeCell ref="R61:U61"/>
-    <mergeCell ref="V61:Y61"/>
-    <mergeCell ref="Z61:AC61"/>
-    <mergeCell ref="AD61:AG61"/>
-    <mergeCell ref="AH61:AK61"/>
-    <mergeCell ref="AL61:AO61"/>
-    <mergeCell ref="AD62:AG62"/>
-    <mergeCell ref="AP64:AS64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="J65:M65"/>
-    <mergeCell ref="N65:Q65"/>
-    <mergeCell ref="R65:U65"/>
-    <mergeCell ref="AP63:AS63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="N64:Q64"/>
-    <mergeCell ref="R64:U64"/>
-    <mergeCell ref="V64:Y64"/>
-    <mergeCell ref="Z64:AC64"/>
-    <mergeCell ref="AH64:AK64"/>
-    <mergeCell ref="AL64:AO64"/>
-    <mergeCell ref="AP66:AS66"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="AD65:AG65"/>
-    <mergeCell ref="AH65:AK65"/>
-    <mergeCell ref="AL65:AO65"/>
-    <mergeCell ref="AP65:AS65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="N66:Q66"/>
-    <mergeCell ref="R66:U66"/>
-    <mergeCell ref="V66:Y66"/>
-    <mergeCell ref="Z66:AC66"/>
-    <mergeCell ref="AD64:AG64"/>
-    <mergeCell ref="AD66:AG66"/>
-    <mergeCell ref="AH66:AK66"/>
-    <mergeCell ref="AL66:AO66"/>
-    <mergeCell ref="V65:Y65"/>
-    <mergeCell ref="Z65:AC65"/>
-    <mergeCell ref="AD63:AG63"/>
-    <mergeCell ref="AH63:AK63"/>
-    <mergeCell ref="AL63:AO63"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="A48:A57"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="D22:D23"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C40:C41"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
     <mergeCell ref="C42:C43"/>
-    <mergeCell ref="E24:E25"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="AH62:AK62"/>
-    <mergeCell ref="AL62:AO62"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>